<commit_message>
[dict] corrections to khaling stories
</commit_message>
<xml_diff>
--- a/corpus/comparable/metadata.xlsx
+++ b/corpus/comparable/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
     <sheet name="update" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="305">
   <si>
     <t>Langue</t>
   </si>
@@ -748,9 +748,6 @@
     <t>TDH-MUKLI_DILWAR.075</t>
   </si>
   <si>
-    <t>53 lignes 'ref' au lieu de 55</t>
-  </si>
-  <si>
     <t>197 lignes 'ref' au lieu de 194</t>
   </si>
   <si>
@@ -841,9 +838,6 @@
     <t>KLR_SOLME1_Dhana.001</t>
   </si>
   <si>
-    <t>KLR_SOLME1_Dhana.055</t>
-  </si>
-  <si>
     <t>KLR_SOLME2_Dhana.001</t>
   </si>
   <si>
@@ -992,6 +986,15 @@
   </si>
   <si>
     <t>TDH-DEUSA_DP_DalBahadur.wav</t>
+  </si>
+  <si>
+    <t>3&amp; that Toolbox can't resolve; otherwise, ready for archiving</t>
+  </si>
+  <si>
+    <t>KLR_SOLME1_Dhana.051</t>
+  </si>
+  <si>
+    <t>2&amp; that TB can't resolve; otherwise READY</t>
   </si>
 </sst>
 </file>
@@ -1427,6 +1430,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1754,11 +1762,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.875" customWidth="1"/>
     <col min="2" max="2" width="58.875" customWidth="1"/>
@@ -1772,7 +1780,7 @@
     <col min="15" max="15" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1">
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1819,18 +1827,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>57</v>
@@ -1848,7 +1856,7 @@
         <v>9</v>
       </c>
       <c r="J2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K2" t="s">
         <v>27</v>
@@ -1866,7 +1874,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="9" t="s">
         <v>82</v>
@@ -1880,27 +1888,27 @@
       <c r="E3" s="9"/>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="N4" s="6"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D5" t="s">
-        <v>253</v>
+        <v>303</v>
       </c>
       <c r="E5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -1930,10 +1938,10 @@
         <v>115</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="9" t="s">
         <v>137</v>
@@ -1952,26 +1960,26 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D8" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
@@ -2001,10 +2009,10 @@
         <v>115</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="9" t="s">
         <v>140</v>
@@ -2019,24 +2027,24 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C11" t="s">
+        <v>254</v>
+      </c>
+      <c r="D11" t="s">
+        <v>255</v>
+      </c>
+      <c r="E11" t="s">
         <v>256</v>
-      </c>
-      <c r="D11" t="s">
-        <v>257</v>
-      </c>
-      <c r="E11" t="s">
-        <v>258</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
@@ -2065,8 +2073,11 @@
       <c r="N11" s="6" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="O11" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="9" t="s">
         <v>143</v>
@@ -2081,7 +2092,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="2" customFormat="1">
+    <row r="13" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -2128,21 +2139,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="E14" t="s">
         <v>283</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="E14" t="s">
-        <v>285</v>
       </c>
       <c r="F14" t="s">
         <v>29</v>
@@ -2172,7 +2183,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="9" t="s">
         <v>106</v>
@@ -2187,26 +2198,26 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="E17" t="s">
         <v>286</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="E17" t="s">
-        <v>288</v>
       </c>
       <c r="F17" t="s">
         <v>29</v>
@@ -2236,7 +2247,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="9" t="s">
         <v>103</v>
@@ -2254,13 +2265,13 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="N19" s="6"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -2304,7 +2315,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="9" t="s">
         <v>134</v>
@@ -2319,24 +2330,24 @@
         <v>199</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F23" t="s">
         <v>29</v>
@@ -2355,21 +2366,21 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C25" t="s">
+        <v>271</v>
+      </c>
+      <c r="D25" t="s">
+        <v>272</v>
+      </c>
+      <c r="E25" t="s">
         <v>273</v>
-      </c>
-      <c r="D25" t="s">
-        <v>274</v>
-      </c>
-      <c r="E25" t="s">
-        <v>275</v>
       </c>
       <c r="F25" t="s">
         <v>53</v>
@@ -2399,7 +2410,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="9" t="s">
         <v>157</v>
@@ -2417,7 +2428,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -2425,7 +2436,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -2433,27 +2444,27 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="N29" s="6"/>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C30" t="s">
+        <v>276</v>
+      </c>
+      <c r="D30" t="s">
+        <v>277</v>
+      </c>
+      <c r="E30" t="s">
         <v>278</v>
-      </c>
-      <c r="D30" t="s">
-        <v>279</v>
-      </c>
-      <c r="E30" t="s">
-        <v>280</v>
       </c>
       <c r="F30" t="s">
         <v>54</v>
@@ -2483,10 +2494,10 @@
         <v>153</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="9" t="s">
         <v>154</v>
@@ -2501,7 +2512,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="2" customFormat="1">
+    <row r="32" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
@@ -2548,21 +2559,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>46</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C33" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="E33" t="s">
         <v>289</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="E33" t="s">
-        <v>291</v>
       </c>
       <c r="F33" t="s">
         <v>45</v>
@@ -2592,10 +2603,10 @@
         <v>81</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="9" t="s">
         <v>97</v>
@@ -2610,26 +2621,26 @@
         <v>216</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>47</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C36" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="E36" t="s">
         <v>292</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="E36" t="s">
-        <v>294</v>
       </c>
       <c r="F36" t="s">
         <v>45</v>
@@ -2659,10 +2670,10 @@
         <v>81</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="9" t="s">
         <v>100</v>
@@ -2680,13 +2691,13 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="N38" s="6"/>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -2724,13 +2735,13 @@
         <v>2011</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N39" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="9" t="s">
         <v>122</v>
@@ -2748,7 +2759,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -2756,26 +2767,26 @@
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C43" t="s">
+        <v>259</v>
+      </c>
+      <c r="D43" t="s">
+        <v>260</v>
+      </c>
+      <c r="E43" t="s">
         <v>261</v>
-      </c>
-      <c r="D43" t="s">
-        <v>262</v>
-      </c>
-      <c r="E43" t="s">
-        <v>263</v>
       </c>
       <c r="F43" t="s">
         <v>45</v>
@@ -2805,7 +2816,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="9" t="s">
         <v>125</v>
@@ -2820,24 +2831,24 @@
         <v>192</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>51</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C46" t="s">
+        <v>262</v>
+      </c>
+      <c r="D46" t="s">
+        <v>263</v>
+      </c>
+      <c r="E46" t="s">
         <v>264</v>
-      </c>
-      <c r="D46" t="s">
-        <v>265</v>
-      </c>
-      <c r="E46" t="s">
-        <v>266</v>
       </c>
       <c r="F46" t="s">
         <v>45</v>
@@ -2867,7 +2878,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="9" t="s">
         <v>116</v>
@@ -2882,7 +2893,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="48" spans="1:15" s="2" customFormat="1">
+    <row r="48" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>6</v>
       </c>
@@ -2929,21 +2940,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>56</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C49" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="E49" t="s">
         <v>295</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="E49" t="s">
-        <v>297</v>
       </c>
       <c r="F49" t="s">
         <v>55</v>
@@ -2973,10 +2984,10 @@
         <v>81</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="9" t="s">
         <v>91</v>
@@ -2991,12 +3002,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -3040,7 +3051,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="9" t="s">
         <v>131</v>
@@ -3055,10 +3066,10 @@
         <v>197</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -3102,7 +3113,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="9" t="s">
         <v>128</v>
@@ -3117,10 +3128,10 @@
         <v>195</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B57" s="3"/>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>60</v>
       </c>
@@ -3164,7 +3175,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="9" t="s">
         <v>160</v>
@@ -3182,7 +3193,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -3190,7 +3201,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -3198,13 +3209,13 @@
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="N62" s="6"/>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -3248,10 +3259,10 @@
         <v>153</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="9" t="s">
         <v>163</v>
@@ -3266,7 +3277,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="65" spans="1:15" s="2" customFormat="1">
+    <row r="65" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>6</v>
       </c>
@@ -3313,7 +3324,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -3354,7 +3365,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
       <c r="B67" s="9" t="s">
         <v>88</v>
@@ -3369,7 +3380,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -3377,13 +3388,13 @@
         <v>113</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="N69" s="6"/>
     </row>
-    <row r="70" spans="1:15" s="2" customFormat="1">
+    <row r="70" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>6</v>
       </c>
@@ -3430,21 +3441,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>66</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C71" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E71" t="s">
         <v>298</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="E71" t="s">
-        <v>300</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>65</v>
@@ -3459,7 +3470,7 @@
         <v>9</v>
       </c>
       <c r="J71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K71" t="s">
         <v>20</v>
@@ -3474,7 +3485,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="9" t="s">
         <v>94</v>
@@ -3492,7 +3503,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -3500,27 +3511,27 @@
         <v>114</v>
       </c>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="N74" s="6"/>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C75" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="E75" t="s">
         <v>301</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="E75" t="s">
-        <v>303</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>65</v>
@@ -3550,10 +3561,10 @@
         <v>81</v>
       </c>
       <c r="O75" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="9" t="s">
         <v>85</v>
@@ -3568,7 +3579,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="77" spans="1:15" s="2" customFormat="1">
+    <row r="77" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>6</v>
       </c>
@@ -3615,21 +3626,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="1:15">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C78" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="E78" t="s">
         <v>267</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="E78" t="s">
-        <v>269</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>70</v>
@@ -3659,7 +3670,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="9" t="s">
         <v>119</v>
@@ -3674,7 +3685,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="80" spans="1:15" s="2" customFormat="1">
+    <row r="80" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>6</v>
       </c>
@@ -3721,21 +3732,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C81" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="E81" s="8" t="s">
         <v>270</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="E81" s="8" t="s">
-        <v>272</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>72</v>
@@ -3765,7 +3776,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="7"/>
       <c r="B82" s="9" t="s">
         <v>146</v>
@@ -3840,22 +3851,22 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="75.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
[corp] change to metadata for comparable corpus files
Name of Dilwar speaker; new story (only recording for now):
ThulungOrigins
</commit_message>
<xml_diff>
--- a/corpus/comparable/metadata.xlsx
+++ b/corpus/comparable/metadata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="309">
   <si>
     <t>Langue</t>
   </si>
@@ -995,6 +995,18 @@
   </si>
   <si>
     <t>2&amp; that TB can't resolve; otherwise READY</t>
+  </si>
+  <si>
+    <t>Thulung origins</t>
+  </si>
+  <si>
+    <t>Settlement of Thulung area</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Recording only</t>
   </si>
 </sst>
 </file>
@@ -1760,10 +1772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O82"/>
+  <dimension ref="A1:O84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3352,6 +3364,12 @@
       <c r="I66" t="s">
         <v>9</v>
       </c>
+      <c r="J66" t="s">
+        <v>245</v>
+      </c>
+      <c r="K66" t="s">
+        <v>20</v>
+      </c>
       <c r="L66">
         <v>2000</v>
       </c>
@@ -3789,6 +3807,32 @@
       </c>
       <c r="E82" s="9" t="s">
         <v>204</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>305</v>
+      </c>
+      <c r="F84" t="s">
+        <v>306</v>
+      </c>
+      <c r="G84" t="s">
+        <v>11</v>
+      </c>
+      <c r="H84" t="s">
+        <v>79</v>
+      </c>
+      <c r="J84" t="s">
+        <v>307</v>
+      </c>
+      <c r="K84" t="s">
+        <v>20</v>
+      </c>
+      <c r="L84">
+        <v>2000</v>
+      </c>
+      <c r="M84" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[corpus] Update 'ref' and 'id' for Dilwar story
</commit_message>
<xml_diff>
--- a/corpus/comparable/metadata.xlsx
+++ b/corpus/comparable/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
     <sheet name="update" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="308">
   <si>
     <t>Langue</t>
   </si>
@@ -229,9 +229,6 @@
     <t>Foundation rites</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>Khamnime</t>
   </si>
   <si>
@@ -295,12 +292,6 @@
     <t>Bina</t>
   </si>
   <si>
-    <t>Where is THU Dilwar?</t>
-  </si>
-  <si>
-    <t>Where is Eagle?</t>
-  </si>
-  <si>
     <t>What additional Koyi/Thulung stories (mythological in nature) can be added (even if not alignable)?</t>
   </si>
   <si>
@@ -616,9 +607,6 @@
     <t>KKT_SJURIME_Mila</t>
   </si>
   <si>
-    <t>TDH-MUKLI_DILWAR</t>
-  </si>
-  <si>
     <t>KLR_ORIGIN_Dhana</t>
   </si>
   <si>
@@ -742,12 +730,6 @@
     <t>KKT_SJURIME_Mila.039</t>
   </si>
   <si>
-    <t>TDH-MUKLI_DILWAR.001</t>
-  </si>
-  <si>
-    <t>TDH-MUKLI_DILWAR.075</t>
-  </si>
-  <si>
     <t>197 lignes 'ref' au lieu de 194</t>
   </si>
   <si>
@@ -1007,6 +989,21 @@
   </si>
   <si>
     <t>Recording only</t>
+  </si>
+  <si>
+    <t>TDH-MUKLI_EAGLE_Bishnu.wav</t>
+  </si>
+  <si>
+    <t>TDH-MUKLI_DILWAR_UttarKumar</t>
+  </si>
+  <si>
+    <t>TDH-MUKLI_DILWAR_UttarKumar.001</t>
+  </si>
+  <si>
+    <t>TDH-MUKLI_DILWAR_UttarKumar.075</t>
+  </si>
+  <si>
+    <t>TDH-MUKLI_DILWAR_UttarKumar.wav</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1083,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="168">
+  <cellStyleXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1255,6 +1252,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1270,7 +1268,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="168">
+  <cellStyles count="169">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -1438,6 +1436,7 @@
     <cellStyle name="Lien hypertexte visité" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1774,11 +1773,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.875" customWidth="1"/>
     <col min="2" max="2" width="58.875" customWidth="1"/>
@@ -1792,7 +1791,7 @@
     <col min="15" max="15" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1833,27 +1832,27 @@
         <v>5</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C2" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D2" t="s">
-        <v>280</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>57</v>
+        <v>274</v>
+      </c>
+      <c r="E2" t="s">
+        <v>303</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -1862,13 +1861,13 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I2" t="s">
         <v>9</v>
       </c>
       <c r="J2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="K2" t="s">
         <v>27</v>
@@ -1880,47 +1879,45 @@
         <v>12</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="7"/>
       <c r="B3" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E3" s="9"/>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="N4" s="6"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="D5" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="E5" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -1947,51 +1944,51 @@
         <v>33</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="7"/>
       <c r="B6" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="B7" s="3"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C8" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D8" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="E8" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
@@ -2015,48 +2012,48 @@
         <v>22</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="7"/>
       <c r="B9" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C11" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D11" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="E11" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
@@ -2083,28 +2080,28 @@
         <v>12</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="7"/>
       <c r="B12" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="2" customFormat="1">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -2145,27 +2142,27 @@
         <v>5</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="E14" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="F14" t="s">
         <v>29</v>
@@ -2174,7 +2171,7 @@
         <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I14" t="s">
         <v>9</v>
@@ -2192,44 +2189,44 @@
         <v>12</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="7"/>
       <c r="B15" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E15" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E17" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="F17" t="s">
         <v>29</v>
@@ -2238,7 +2235,7 @@
         <v>11</v>
       </c>
       <c r="H17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I17" t="s">
         <v>9</v>
@@ -2256,48 +2253,48 @@
         <v>34</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="7"/>
       <c r="B18" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E18" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="N19" s="6"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C20" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D20" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E20" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F20" t="s">
         <v>29</v>
@@ -2324,42 +2321,42 @@
         <v>12</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="7"/>
       <c r="B21" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="F23" t="s">
         <v>29</v>
@@ -2378,21 +2375,21 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C25" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D25" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E25" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F25" t="s">
         <v>53</v>
@@ -2419,64 +2416,64 @@
         <v>41</v>
       </c>
       <c r="N25" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="7"/>
       <c r="B26" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="N27" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="N28" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="N29" s="6"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
         <v>42</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C30" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D30" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="E30" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="F30" t="s">
         <v>54</v>
@@ -2503,28 +2500,28 @@
         <v>12</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="7"/>
       <c r="B31" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E31" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" s="2" customFormat="1">
       <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
@@ -2565,27 +2562,27 @@
         <v>5</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="O32" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>46</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E33" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="F33" t="s">
         <v>45</v>
@@ -2594,7 +2591,7 @@
         <v>11</v>
       </c>
       <c r="H33" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I33" t="s">
         <v>9</v>
@@ -2612,47 +2609,47 @@
         <v>12</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="7"/>
       <c r="B34" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E34" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>47</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="E36" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F36" t="s">
         <v>45</v>
@@ -2661,7 +2658,7 @@
         <v>11</v>
       </c>
       <c r="H36" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I36" t="s">
         <v>9</v>
@@ -2679,51 +2676,51 @@
         <v>48</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" s="7"/>
       <c r="B37" s="9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="N38" s="6"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>49</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F39" t="s">
         <v>45</v>
@@ -2747,58 +2744,58 @@
         <v>2011</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" s="7"/>
       <c r="B40" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="N41" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
         <v>49</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C43" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D43" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E43" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F43" t="s">
         <v>45</v>
@@ -2825,42 +2822,42 @@
         <v>12</v>
       </c>
       <c r="N43" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" s="7"/>
       <c r="B44" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
         <v>51</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C46" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D46" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E46" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="F46" t="s">
         <v>45</v>
@@ -2887,25 +2884,25 @@
         <v>12</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" s="7"/>
       <c r="B47" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" s="2" customFormat="1">
       <c r="A48" s="2" t="s">
         <v>6</v>
       </c>
@@ -2946,27 +2943,27 @@
         <v>5</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="O48" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15">
       <c r="A49" t="s">
         <v>56</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="E49" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="F49" t="s">
         <v>55</v>
@@ -2975,7 +2972,7 @@
         <v>11</v>
       </c>
       <c r="H49" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I49" t="s">
         <v>9</v>
@@ -2993,47 +2990,47 @@
         <v>12</v>
       </c>
       <c r="N49" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" s="7"/>
       <c r="B50" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E50" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E52" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F52" t="s">
         <v>55</v>
@@ -3048,7 +3045,7 @@
         <v>9</v>
       </c>
       <c r="J52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K52" t="s">
         <v>20</v>
@@ -3060,42 +3057,42 @@
         <v>12</v>
       </c>
       <c r="N52" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53" s="7"/>
       <c r="B53" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E55" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F55" t="s">
         <v>55</v>
@@ -3122,42 +3119,42 @@
         <v>12</v>
       </c>
       <c r="N55" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
       <c r="A56" s="7"/>
       <c r="B56" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
       <c r="B57" s="3"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E58" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F58" t="s">
         <v>55</v>
@@ -3181,67 +3178,67 @@
         <v>2009</v>
       </c>
       <c r="M58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N58" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" s="7"/>
       <c r="B59" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E59" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="N59" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="N60" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="N61" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="N62" s="6"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C63" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D63" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E63" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F63" t="s">
         <v>55</v>
@@ -3268,28 +3265,28 @@
         <v>12</v>
       </c>
       <c r="N63" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
       <c r="A64" s="7"/>
       <c r="B64" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" s="2" customFormat="1">
       <c r="A65" s="2" t="s">
         <v>6</v>
       </c>
@@ -3330,42 +3327,42 @@
         <v>5</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="O65" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15">
       <c r="A66" t="s">
-        <v>64</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>307</v>
       </c>
       <c r="F66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G66" t="s">
         <v>11</v>
       </c>
       <c r="H66" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I66" t="s">
         <v>9</v>
       </c>
       <c r="J66" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="K66" t="s">
         <v>20</v>
@@ -3377,42 +3374,40 @@
         <v>12</v>
       </c>
       <c r="N66" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="O66" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="O66" s="4"/>
+    </row>
+    <row r="67" spans="1:15">
       <c r="A67" s="7"/>
       <c r="B67" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N67" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="N68" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="N69" s="6"/>
     </row>
-    <row r="70" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" s="2" customFormat="1">
       <c r="A70" s="2" t="s">
         <v>6</v>
       </c>
@@ -3453,42 +3448,42 @@
         <v>5</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="O70" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E71" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G71" t="s">
         <v>11</v>
       </c>
       <c r="H71" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I71" t="s">
         <v>9</v>
       </c>
       <c r="J71" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="K71" t="s">
         <v>20</v>
@@ -3497,74 +3492,74 @@
         <v>2000</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N71" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15">
       <c r="A72" s="7"/>
       <c r="B72" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E72" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="N72" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15">
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="N73" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15">
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="N74" s="6"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15">
       <c r="A75" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="E75" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G75" t="s">
         <v>11</v>
       </c>
       <c r="H75" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I75" t="s">
         <v>9</v>
       </c>
       <c r="J75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K75" t="s">
         <v>20</v>
@@ -3576,28 +3571,28 @@
         <v>12</v>
       </c>
       <c r="N75" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O75" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15">
       <c r="A76" s="7"/>
       <c r="B76" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" s="2" customFormat="1">
       <c r="A77" s="2" t="s">
         <v>6</v>
       </c>
@@ -3638,30 +3633,30 @@
         <v>5</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="O77" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15">
       <c r="A78" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="E78" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G78" t="s">
         <v>21</v>
@@ -3682,28 +3677,28 @@
         <v>28</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N78" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
       <c r="A79" s="7"/>
       <c r="B79" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" s="2" customFormat="1">
       <c r="A80" s="2" t="s">
         <v>6</v>
       </c>
@@ -3744,30 +3739,30 @@
         <v>5</v>
       </c>
       <c r="N80" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="O80" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14">
       <c r="A81" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G81" t="s">
         <v>21</v>
@@ -3779,7 +3774,7 @@
         <v>9</v>
       </c>
       <c r="J81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K81" t="s">
         <v>27</v>
@@ -3788,42 +3783,42 @@
         <v>28</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N81" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14">
       <c r="A82" s="7"/>
       <c r="B82" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14">
       <c r="A84" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="F84" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="G84" t="s">
         <v>11</v>
       </c>
       <c r="H84" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J84" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="K84" t="s">
         <v>20</v>
@@ -3832,7 +3827,7 @@
         <v>2000</v>
       </c>
       <c r="M84" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -3895,24 +3890,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="75.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[dict] revision of Solme Lamalit Khaling
also changes to metadata file
</commit_message>
<xml_diff>
--- a/corpus/comparable/metadata.xlsx
+++ b/corpus/comparable/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
     <sheet name="update" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="306">
   <si>
     <t>Langue</t>
   </si>
@@ -119,21 +119,6 @@
   </si>
   <si>
     <t>Lakpa</t>
-  </si>
-  <si>
-    <r>
-      <t>Toolbox</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> but only transcription and glossing</t>
-    </r>
   </si>
   <si>
     <r>
@@ -517,21 +502,6 @@
     <t>https://github.com/CNRS/HimalCo/blob/master/corpus/khaling/toolbox/KHASolmeLamalit.txt</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Toolbox </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>but only transcription and glossing, no translation</t>
-    </r>
-  </si>
-  <si>
     <t>https://github.com/CNRS/HimalCo/blob/master/dict/koyi/toolbox/Texts.txt</t>
   </si>
   <si>
@@ -730,9 +700,6 @@
     <t>KKT_SJURIME_Mila.039</t>
   </si>
   <si>
-    <t>197 lignes 'ref' au lieu de 194</t>
-  </si>
-  <si>
     <t>108 lignes 'ref' au lieu de 105</t>
   </si>
   <si>
@@ -823,9 +790,6 @@
     <t>KLR_SOLME2_Dhana.001</t>
   </si>
   <si>
-    <t>KLR_SOLME2_Dhana.194</t>
-  </si>
-  <si>
     <t>KLR_SOLME_DhanMaya.001</t>
   </si>
   <si>
@@ -970,15 +934,9 @@
     <t>TDH-DEUSA_DP_DalBahadur.wav</t>
   </si>
   <si>
-    <t>3&amp; that Toolbox can't resolve; otherwise, ready for archiving</t>
-  </si>
-  <si>
     <t>KLR_SOLME1_Dhana.051</t>
   </si>
   <si>
-    <t>2&amp; that TB can't resolve; otherwise READY</t>
-  </si>
-  <si>
     <t>Thulung origins</t>
   </si>
   <si>
@@ -1004,6 +962,18 @@
   </si>
   <si>
     <t>TDH-MUKLI_DILWAR_UttarKumar.wav</t>
+  </si>
+  <si>
+    <t>KLR_SOLME2_Dhana.163</t>
+  </si>
+  <si>
+    <t>2&amp; that TB can't resolve; otherwise READY (but check against recording)</t>
+  </si>
+  <si>
+    <t>Some &amp; that TB can't resolve, otherwise READY (but check against recording)</t>
+  </si>
+  <si>
+    <t>3&amp; that Toolbox can't resolve; otherwise, ready for archiving (but check against recording)</t>
   </si>
 </sst>
 </file>
@@ -1773,11 +1743,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.875" customWidth="1"/>
     <col min="2" max="2" width="58.875" customWidth="1"/>
@@ -1791,7 +1759,7 @@
     <col min="15" max="15" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1">
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1832,27 +1800,27 @@
         <v>5</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E2" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -1861,13 +1829,13 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I2" t="s">
         <v>9</v>
       </c>
       <c r="J2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="K2" t="s">
         <v>27</v>
@@ -1879,45 +1847,45 @@
         <v>12</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>81</v>
       </c>
       <c r="E3" s="9"/>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="N4" s="6"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -1941,54 +1909,54 @@
         <v>22</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>136</v>
-      </c>
       <c r="E6" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D8" t="s">
+        <v>302</v>
+      </c>
+      <c r="E8" t="s">
         <v>247</v>
-      </c>
-      <c r="E8" t="s">
-        <v>251</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
@@ -2012,48 +1980,48 @@
         <v>22</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>149</v>
+        <v>12</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>139</v>
-      </c>
       <c r="E9" s="9" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C11" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D11" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E11" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
@@ -2080,28 +2048,28 @@
         <v>12</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>142</v>
-      </c>
       <c r="E12" s="9" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" s="2" customFormat="1">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -2142,27 +2110,27 @@
         <v>5</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E14" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F14" t="s">
         <v>29</v>
@@ -2171,7 +2139,7 @@
         <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I14" t="s">
         <v>9</v>
@@ -2189,44 +2157,44 @@
         <v>12</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>105</v>
-      </c>
       <c r="E15" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E17" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F17" t="s">
         <v>29</v>
@@ -2235,7 +2203,7 @@
         <v>11</v>
       </c>
       <c r="H17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I17" t="s">
         <v>9</v>
@@ -2250,51 +2218,51 @@
         <v>2009</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>102</v>
-      </c>
       <c r="E18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="N19" s="6"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" t="s">
+        <v>174</v>
+      </c>
+      <c r="D20" t="s">
         <v>175</v>
       </c>
-      <c r="C20" t="s">
-        <v>176</v>
-      </c>
-      <c r="D20" t="s">
-        <v>177</v>
-      </c>
       <c r="E20" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F20" t="s">
         <v>29</v>
@@ -2315,48 +2283,48 @@
         <v>20</v>
       </c>
       <c r="L20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M20" t="s">
         <v>12</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="D21" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>133</v>
-      </c>
       <c r="E21" s="9" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F23" t="s">
         <v>29</v>
@@ -2368,34 +2336,34 @@
         <v>25</v>
       </c>
       <c r="I23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N23" s="6"/>
       <c r="O23" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C25" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D25" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E25" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H25" t="s">
         <v>25</v>
@@ -2404,7 +2372,7 @@
         <v>9</v>
       </c>
       <c r="J25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K25" t="s">
         <v>20</v>
@@ -2413,73 +2381,73 @@
         <v>2004</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N25" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>156</v>
-      </c>
       <c r="E26" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="N27" s="6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="N28" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="N29" s="6"/>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C30" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D30" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E30" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H30" t="s">
         <v>25</v>
@@ -2488,40 +2456,40 @@
         <v>9</v>
       </c>
       <c r="J30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K30" t="s">
         <v>27</v>
       </c>
       <c r="L30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M30" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>153</v>
-      </c>
       <c r="E31" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" s="2" customFormat="1">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
@@ -2562,36 +2530,36 @@
         <v>5</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E33" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G33" t="s">
         <v>11</v>
       </c>
       <c r="H33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I33" t="s">
         <v>9</v>
@@ -2609,56 +2577,56 @@
         <v>12</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="D34" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D34" s="9" t="s">
-        <v>96</v>
-      </c>
       <c r="E34" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E36" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G36" t="s">
         <v>11</v>
       </c>
       <c r="H36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I36" t="s">
         <v>9</v>
@@ -2673,57 +2641,57 @@
         <v>2009</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="D37" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>99</v>
-      </c>
       <c r="E37" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="N38" s="6"/>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G39" t="s">
         <v>21</v>
@@ -2744,61 +2712,61 @@
         <v>2011</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="D40" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>121</v>
-      </c>
       <c r="E40" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="N41" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C43" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D43" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E43" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G43" t="s">
         <v>21</v>
@@ -2810,7 +2778,7 @@
         <v>9</v>
       </c>
       <c r="J43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K43" t="s">
         <v>20</v>
@@ -2822,45 +2790,45 @@
         <v>12</v>
       </c>
       <c r="N43" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="D44" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>124</v>
-      </c>
       <c r="E44" s="9" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C46" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D46" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E46" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G46" t="s">
         <v>21</v>
@@ -2872,7 +2840,7 @@
         <v>9</v>
       </c>
       <c r="J46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K46" t="s">
         <v>20</v>
@@ -2884,25 +2852,25 @@
         <v>12</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="D47" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D47" s="9" t="s">
-        <v>115</v>
-      </c>
       <c r="E47" s="9" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" s="2" customFormat="1">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>6</v>
       </c>
@@ -2943,36 +2911,36 @@
         <v>5</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E49" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G49" t="s">
         <v>11</v>
       </c>
       <c r="H49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I49" t="s">
         <v>9</v>
@@ -2990,50 +2958,50 @@
         <v>12</v>
       </c>
       <c r="N49" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="D50" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D50" s="9" t="s">
-        <v>90</v>
-      </c>
       <c r="E50" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E52" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G52" t="s">
         <v>21</v>
@@ -3045,7 +3013,7 @@
         <v>9</v>
       </c>
       <c r="J52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K52" t="s">
         <v>20</v>
@@ -3057,45 +3025,45 @@
         <v>12</v>
       </c>
       <c r="N52" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="D53" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="D53" s="9" t="s">
-        <v>130</v>
-      </c>
       <c r="E53" s="9" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E55" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G55" t="s">
         <v>21</v>
@@ -3107,7 +3075,7 @@
         <v>9</v>
       </c>
       <c r="J55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K55" t="s">
         <v>20</v>
@@ -3119,48 +3087,48 @@
         <v>12</v>
       </c>
       <c r="N55" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="D56" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D56" s="9" t="s">
-        <v>127</v>
-      </c>
       <c r="E56" s="9" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B57" s="3"/>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E58" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G58" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H58" t="s">
         <v>25</v>
@@ -3169,7 +3137,7 @@
         <v>9</v>
       </c>
       <c r="J58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K58" t="s">
         <v>20</v>
@@ -3178,73 +3146,73 @@
         <v>2009</v>
       </c>
       <c r="M58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N58" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D59" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C59" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>159</v>
-      </c>
       <c r="E59" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="N59" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="N60" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="N61" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="N62" s="6"/>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C63" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D63" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E63" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F63" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H63" t="s">
         <v>25</v>
@@ -3253,40 +3221,40 @@
         <v>9</v>
       </c>
       <c r="J63" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K63" t="s">
         <v>27</v>
       </c>
       <c r="L63" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M63" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N63" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="D64" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="C64" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>162</v>
-      </c>
       <c r="E64" s="8" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" s="2" customFormat="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>6</v>
       </c>
@@ -3327,42 +3295,42 @@
         <v>5</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="O65" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="F66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G66" t="s">
         <v>11</v>
       </c>
       <c r="H66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I66" t="s">
         <v>9</v>
       </c>
       <c r="J66" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K66" t="s">
         <v>20</v>
@@ -3374,40 +3342,40 @@
         <v>12</v>
       </c>
       <c r="N66" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O66" s="4"/>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
       <c r="B67" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="D67" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D67" s="9" t="s">
-        <v>87</v>
-      </c>
       <c r="N67" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="N68" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="N69" s="6"/>
     </row>
-    <row r="70" spans="1:15" s="2" customFormat="1">
+    <row r="70" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>6</v>
       </c>
@@ -3448,42 +3416,42 @@
         <v>5</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E71" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G71" t="s">
         <v>11</v>
       </c>
       <c r="H71" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I71" t="s">
         <v>9</v>
       </c>
       <c r="J71" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K71" t="s">
         <v>20</v>
@@ -3492,74 +3460,74 @@
         <v>2000</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N71" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C72" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C72" s="9" t="s">
+      <c r="D72" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D72" s="9" t="s">
-        <v>93</v>
-      </c>
       <c r="E72" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="N72" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="N73" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="N74" s="6"/>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E75" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G75" t="s">
         <v>11</v>
       </c>
       <c r="H75" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I75" t="s">
         <v>9</v>
       </c>
       <c r="J75" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K75" t="s">
         <v>20</v>
@@ -3571,28 +3539,28 @@
         <v>12</v>
       </c>
       <c r="N75" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O75" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C76" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="D76" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D76" s="9" t="s">
-        <v>84</v>
-      </c>
       <c r="E76" s="8" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" s="2" customFormat="1">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>6</v>
       </c>
@@ -3633,30 +3601,30 @@
         <v>5</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="O77" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E78" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G78" t="s">
         <v>21</v>
@@ -3677,28 +3645,28 @@
         <v>28</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N78" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C79" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C79" s="9" t="s">
+      <c r="D79" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D79" s="9" t="s">
-        <v>118</v>
-      </c>
       <c r="E79" s="9" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" s="2" customFormat="1">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>6</v>
       </c>
@@ -3739,30 +3707,30 @@
         <v>5</v>
       </c>
       <c r="N80" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="O80" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G81" t="s">
         <v>21</v>
@@ -3774,7 +3742,7 @@
         <v>9</v>
       </c>
       <c r="J81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K81" t="s">
         <v>27</v>
@@ -3783,42 +3751,42 @@
         <v>28</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N81" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="7"/>
       <c r="B82" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C82" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C82" s="9" t="s">
+      <c r="D82" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="D82" s="9" t="s">
-        <v>145</v>
-      </c>
       <c r="E82" s="9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="F84" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="G84" t="s">
         <v>11</v>
       </c>
       <c r="H84" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J84" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="K84" t="s">
         <v>20</v>
@@ -3827,7 +3795,7 @@
         <v>2000</v>
       </c>
       <c r="M84" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -3890,24 +3858,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="75.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[corpus] Update matadata (meeting with Séverine)
</commit_message>
<xml_diff>
--- a/corpus/comparable/metadata.xlsx
+++ b/corpus/comparable/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
     <sheet name="update" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="301">
   <si>
     <t>Langue</t>
   </si>
@@ -457,24 +457,6 @@
     <t>origin.121</t>
   </si>
   <si>
-    <t>SolmeLamalit 1/2 (Dhana, June 2011)</t>
-  </si>
-  <si>
-    <t>solme.001</t>
-  </si>
-  <si>
-    <t>solme.055</t>
-  </si>
-  <si>
-    <t>SolmeLamalit 2/2 (Dhana, June 2011)</t>
-  </si>
-  <si>
-    <t>solme2.001</t>
-  </si>
-  <si>
-    <t>solme2.194</t>
-  </si>
-  <si>
     <t>SolmeLamalit (Dhan Maya, rec Oct 2014) [rechecked]</t>
   </si>
   <si>
@@ -643,12 +625,6 @@
     <t>KLR_ORIGIN_Dhana.wav</t>
   </si>
   <si>
-    <t>KHA_SolmeLamalit_Dhana_Jun2011.WAV</t>
-  </si>
-  <si>
-    <t>KHA_SolmeLamalit_PtII_Dhana_Jun2011.wav</t>
-  </si>
-  <si>
     <t>KHA_SolmeLamalit_DhanMaya_Oct2014.wav</t>
   </si>
   <si>
@@ -781,9 +757,6 @@
     <t>ITE but mistakes, ask GJ</t>
   </si>
   <si>
-    <t>Friday 27 March 2015</t>
-  </si>
-  <si>
     <t>KLR_SOLME1_Dhana.001</t>
   </si>
   <si>
@@ -974,6 +947,18 @@
   </si>
   <si>
     <t>3&amp; that Toolbox can't resolve; otherwise, ready for archiving (but check against recording)</t>
+  </si>
+  <si>
+    <t>Lieu</t>
+  </si>
+  <si>
+    <t>Katmandou</t>
+  </si>
+  <si>
+    <t>Phuleli</t>
+  </si>
+  <si>
+    <t>Friday 17 April 2015</t>
   </si>
 </sst>
 </file>
@@ -986,6 +971,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1053,7 +1039,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="169">
+  <cellStyleXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1222,6 +1208,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
@@ -1238,7 +1226,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="169">
+  <cellStyles count="171">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -1407,6 +1395,8 @@
     <cellStyle name="Lien hypertexte visité" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1741,11 +1731,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O84"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.875" customWidth="1"/>
     <col min="2" max="2" width="58.875" customWidth="1"/>
@@ -1754,12 +1746,12 @@
     <col min="6" max="6" width="24.875" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
     <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="13" max="13" width="63" customWidth="1"/>
-    <col min="14" max="14" width="85.625" customWidth="1"/>
-    <col min="15" max="15" width="24.5" customWidth="1"/>
+    <col min="14" max="14" width="63" customWidth="1"/>
+    <col min="15" max="15" width="85.625" customWidth="1"/>
+    <col min="16" max="16" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1797,30 +1789,33 @@
         <v>4</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="O1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C2" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="D2" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="E2" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -1835,7 +1830,7 @@
         <v>9</v>
       </c>
       <c r="J2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K2" t="s">
         <v>27</v>
@@ -1843,15 +1838,18 @@
       <c r="L2">
         <v>2000</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" t="s">
+        <v>298</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="4"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" s="4"/>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="7"/>
       <c r="B3" s="9" t="s">
         <v>78</v>
@@ -1863,29 +1861,29 @@
         <v>80</v>
       </c>
       <c r="E3" s="9"/>
-      <c r="N3" s="6"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="1:16">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="N4" s="6"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O4" s="6"/>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C5" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="E5" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -1908,55 +1906,50 @@
       <c r="L5" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" t="s">
+        <v>298</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="O5" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="O5" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="7"/>
-      <c r="B6" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="M6" s="1"/>
-      <c r="N6" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="B7" s="3"/>
-      <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C8" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="D8" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="E8" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
@@ -1979,1866 +1972,1920 @@
       <c r="L8" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" t="s">
+        <v>298</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="O8" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="O8" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="P8" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="C11" t="s">
-        <v>244</v>
-      </c>
-      <c r="D11" t="s">
-        <v>245</v>
-      </c>
-      <c r="E11" t="s">
-        <v>246</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="B10" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" t="s">
+        <v>235</v>
+      </c>
+      <c r="D10" t="s">
+        <v>236</v>
+      </c>
+      <c r="E10" t="s">
+        <v>237</v>
+      </c>
+      <c r="F10" t="s">
         <v>10</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G10" t="s">
         <v>21</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H10" t="s">
         <v>25</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I10" t="s">
         <v>9</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J10" t="s">
         <v>26</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K10" t="s">
         <v>27</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L10" t="s">
         <v>28</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="M10" t="s">
+        <v>298</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N11" s="6" t="s">
+      <c r="O10" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="O11" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="P10" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="7"/>
+      <c r="B11" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="2" customFormat="1">
+      <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="N12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="O12" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E13" t="s">
+        <v>264</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13">
+        <v>2014</v>
+      </c>
+      <c r="M13" t="s">
+        <v>298</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="7"/>
+      <c r="B14" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="E16" t="s">
+        <v>267</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" t="s">
+        <v>76</v>
+      </c>
+      <c r="I16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16">
+        <v>2009</v>
+      </c>
+      <c r="M16" t="s">
+        <v>298</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="7"/>
+      <c r="B17" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" t="s">
+        <v>198</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="O18" s="6"/>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
         <v>167</v>
       </c>
-      <c r="O13" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="E14" t="s">
-        <v>273</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="C19" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19" t="s">
+        <v>169</v>
+      </c>
+      <c r="E19" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" t="s">
         <v>29</v>
       </c>
-      <c r="G14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" t="s">
-        <v>75</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" t="s">
         <v>9</v>
       </c>
-      <c r="J14" t="s">
-        <v>31</v>
-      </c>
-      <c r="K14" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14">
-        <v>2014</v>
-      </c>
-      <c r="M14" s="1" t="s">
+      <c r="J19" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" t="s">
+        <v>42</v>
+      </c>
+      <c r="M19" t="s">
+        <v>298</v>
+      </c>
+      <c r="N19" t="s">
         <v>12</v>
       </c>
-      <c r="N14" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E15" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="E17" t="s">
-        <v>276</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="O19" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="7"/>
+      <c r="B20" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="F22" t="s">
         <v>29</v>
       </c>
-      <c r="G17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="G22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" t="s">
+        <v>35</v>
+      </c>
+      <c r="O22" s="6"/>
+      <c r="P22" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C24" t="s">
+        <v>252</v>
+      </c>
+      <c r="D24" t="s">
+        <v>253</v>
+      </c>
+      <c r="E24" t="s">
+        <v>254</v>
+      </c>
+      <c r="F24" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" t="s">
         <v>9</v>
       </c>
-      <c r="J17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K17" t="s">
+      <c r="J24" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" t="s">
         <v>20</v>
       </c>
-      <c r="L17">
-        <v>2009</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" t="s">
-        <v>206</v>
-      </c>
-      <c r="N18" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="N19" s="6"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" t="s">
-        <v>173</v>
-      </c>
-      <c r="C20" t="s">
-        <v>174</v>
-      </c>
-      <c r="D20" t="s">
-        <v>175</v>
-      </c>
-      <c r="E20" t="s">
-        <v>194</v>
-      </c>
-      <c r="F20" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20" t="s">
-        <v>19</v>
-      </c>
-      <c r="K20" t="s">
-        <v>20</v>
-      </c>
-      <c r="L20" t="s">
-        <v>42</v>
-      </c>
-      <c r="M20" t="s">
-        <v>12</v>
-      </c>
-      <c r="N20" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="F23" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I23" t="s">
-        <v>35</v>
-      </c>
-      <c r="N23" s="6"/>
-      <c r="O23" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C25" t="s">
-        <v>261</v>
-      </c>
-      <c r="D25" t="s">
-        <v>262</v>
-      </c>
-      <c r="E25" t="s">
-        <v>263</v>
-      </c>
-      <c r="F25" t="s">
-        <v>52</v>
-      </c>
-      <c r="G25" t="s">
-        <v>38</v>
-      </c>
-      <c r="H25" t="s">
-        <v>25</v>
-      </c>
-      <c r="I25" t="s">
-        <v>9</v>
-      </c>
-      <c r="J25" t="s">
-        <v>39</v>
-      </c>
-      <c r="K25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25">
+      <c r="L24">
         <v>2004</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="M24" t="s">
+        <v>298</v>
+      </c>
+      <c r="N24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N25" s="6" t="s">
+      <c r="O24" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="7"/>
+      <c r="B25" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="N26" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E25" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="O26" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="N27" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O27" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="N28" s="6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="N29" s="6"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="O28" s="6"/>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="C30" t="s">
-        <v>266</v>
-      </c>
-      <c r="D30" t="s">
-        <v>267</v>
+      <c r="B29" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C29" t="s">
+        <v>257</v>
+      </c>
+      <c r="D29" t="s">
+        <v>258</v>
+      </c>
+      <c r="E29" t="s">
+        <v>259</v>
+      </c>
+      <c r="F29" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" t="s">
+        <v>38</v>
+      </c>
+      <c r="H29" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" t="s">
+        <v>43</v>
+      </c>
+      <c r="K29" t="s">
+        <v>27</v>
+      </c>
+      <c r="L29" t="s">
+        <v>42</v>
+      </c>
+      <c r="M29" t="s">
+        <v>298</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="7"/>
+      <c r="B30" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>145</v>
       </c>
       <c r="E30" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" s="2" customFormat="1">
+      <c r="A31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="F30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G30" t="s">
-        <v>38</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="D32" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="E32" t="s">
+        <v>270</v>
+      </c>
+      <c r="F32" t="s">
+        <v>44</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J32" t="s">
+        <v>31</v>
+      </c>
+      <c r="K32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L32">
+        <v>2014</v>
+      </c>
+      <c r="M32" t="s">
+        <v>298</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O32" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="P32" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="7"/>
+      <c r="B33" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="E35" t="s">
+        <v>273</v>
+      </c>
+      <c r="F35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" t="s">
+        <v>76</v>
+      </c>
+      <c r="I35" t="s">
+        <v>9</v>
+      </c>
+      <c r="J35" t="s">
+        <v>32</v>
+      </c>
+      <c r="K35" t="s">
+        <v>20</v>
+      </c>
+      <c r="L35">
+        <v>2009</v>
+      </c>
+      <c r="M35" t="s">
+        <v>298</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="P35" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" s="7"/>
+      <c r="B36" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="O37" s="6"/>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="F38" t="s">
+        <v>44</v>
+      </c>
+      <c r="G38" t="s">
+        <v>21</v>
+      </c>
+      <c r="H38" t="s">
         <v>25</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I38" t="s">
         <v>9</v>
       </c>
-      <c r="J30" t="s">
-        <v>43</v>
-      </c>
-      <c r="K30" t="s">
-        <v>27</v>
-      </c>
-      <c r="L30" t="s">
-        <v>42</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N30" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="O30" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="E31" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="O32" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="E33" t="s">
-        <v>279</v>
-      </c>
-      <c r="F33" t="s">
-        <v>44</v>
-      </c>
-      <c r="G33" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" t="s">
-        <v>75</v>
-      </c>
-      <c r="I33" t="s">
-        <v>9</v>
-      </c>
-      <c r="J33" t="s">
-        <v>31</v>
-      </c>
-      <c r="K33" t="s">
-        <v>27</v>
-      </c>
-      <c r="L33">
-        <v>2014</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N33" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O33" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="E34" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="E36" t="s">
-        <v>282</v>
-      </c>
-      <c r="F36" t="s">
-        <v>44</v>
-      </c>
-      <c r="G36" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" t="s">
-        <v>76</v>
-      </c>
-      <c r="I36" t="s">
-        <v>9</v>
-      </c>
-      <c r="J36" t="s">
-        <v>32</v>
-      </c>
-      <c r="K36" t="s">
+      <c r="J38" t="s">
+        <v>19</v>
+      </c>
+      <c r="K38" t="s">
         <v>20</v>
       </c>
-      <c r="L36">
-        <v>2009</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N36" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O36" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="N37" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="N38" s="6"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="F39" t="s">
-        <v>44</v>
-      </c>
-      <c r="G39" t="s">
-        <v>21</v>
-      </c>
-      <c r="H39" t="s">
-        <v>25</v>
-      </c>
-      <c r="I39" t="s">
-        <v>9</v>
-      </c>
-      <c r="J39" t="s">
-        <v>19</v>
-      </c>
-      <c r="K39" t="s">
-        <v>20</v>
-      </c>
-      <c r="L39">
+      <c r="L38">
         <v>2011</v>
       </c>
-      <c r="M39" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="N39" s="6" t="s">
+      <c r="M38" t="s">
+        <v>298</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="O38" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="9" t="s">
+    <row r="39" spans="1:16">
+      <c r="A39" s="7"/>
+      <c r="B39" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C39" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D39" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E40" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="N40" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E39" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="O39" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="O40" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
-      <c r="N41" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="C43" t="s">
-        <v>249</v>
-      </c>
-      <c r="D43" t="s">
-        <v>250</v>
-      </c>
-      <c r="E43" t="s">
-        <v>251</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="B42" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C42" t="s">
+        <v>240</v>
+      </c>
+      <c r="D42" t="s">
+        <v>241</v>
+      </c>
+      <c r="E42" t="s">
+        <v>242</v>
+      </c>
+      <c r="F42" t="s">
         <v>44</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G42" t="s">
         <v>21</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H42" t="s">
         <v>25</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I42" t="s">
         <v>9</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J42" t="s">
         <v>49</v>
       </c>
-      <c r="K43" t="s">
+      <c r="K42" t="s">
         <v>20</v>
       </c>
-      <c r="L43">
+      <c r="L42">
         <v>2013</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="M42" t="s">
+        <v>299</v>
+      </c>
+      <c r="N42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N43" s="6" t="s">
+      <c r="O42" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="9" t="s">
+    <row r="43" spans="1:16">
+      <c r="A43" s="7"/>
+      <c r="B43" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C43" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D43" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E43" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="C45" t="s">
+        <v>243</v>
+      </c>
+      <c r="D45" t="s">
+        <v>244</v>
+      </c>
+      <c r="E45" t="s">
+        <v>245</v>
+      </c>
+      <c r="F45" t="s">
+        <v>44</v>
+      </c>
+      <c r="G45" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" t="s">
+        <v>25</v>
+      </c>
+      <c r="I45" t="s">
+        <v>9</v>
+      </c>
+      <c r="J45" t="s">
+        <v>51</v>
+      </c>
+      <c r="K45" t="s">
+        <v>20</v>
+      </c>
+      <c r="L45">
+        <v>2013</v>
+      </c>
+      <c r="M45" t="s">
+        <v>298</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O45" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" s="7"/>
+      <c r="B46" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" s="2" customFormat="1">
+      <c r="A47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O47" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="E48" t="s">
+        <v>276</v>
+      </c>
+      <c r="F48" t="s">
+        <v>54</v>
+      </c>
+      <c r="G48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" t="s">
+        <v>75</v>
+      </c>
+      <c r="I48" t="s">
+        <v>9</v>
+      </c>
+      <c r="J48" t="s">
+        <v>31</v>
+      </c>
+      <c r="K48" t="s">
+        <v>27</v>
+      </c>
+      <c r="L48">
+        <v>2014</v>
+      </c>
+      <c r="M48" t="s">
+        <v>298</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O48" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="P48" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="A49" s="7"/>
+      <c r="B49" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E49" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E51" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="3"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="C46" t="s">
-        <v>252</v>
-      </c>
-      <c r="D46" t="s">
-        <v>253</v>
-      </c>
-      <c r="E46" t="s">
-        <v>254</v>
-      </c>
-      <c r="F46" t="s">
-        <v>44</v>
-      </c>
-      <c r="G46" t="s">
+      <c r="F51" t="s">
+        <v>54</v>
+      </c>
+      <c r="G51" t="s">
         <v>21</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H51" t="s">
         <v>25</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I51" t="s">
         <v>9</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J51" t="s">
+        <v>57</v>
+      </c>
+      <c r="K51" t="s">
+        <v>20</v>
+      </c>
+      <c r="L51">
+        <v>2013</v>
+      </c>
+      <c r="M51" t="s">
+        <v>298</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O51" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="A52" s="7"/>
+      <c r="B52" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="A54" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E54" t="s">
+        <v>184</v>
+      </c>
+      <c r="F54" t="s">
+        <v>54</v>
+      </c>
+      <c r="G54" t="s">
+        <v>21</v>
+      </c>
+      <c r="H54" t="s">
+        <v>25</v>
+      </c>
+      <c r="I54" t="s">
+        <v>9</v>
+      </c>
+      <c r="J54" t="s">
         <v>51</v>
       </c>
-      <c r="K46" t="s">
+      <c r="K54" t="s">
         <v>20</v>
       </c>
-      <c r="L46">
+      <c r="L54">
         <v>2013</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="M54" t="s">
+        <v>298</v>
+      </c>
+      <c r="N54" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N46" s="6" t="s">
+      <c r="O54" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L48" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M48" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N48" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="O48" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="E49" t="s">
-        <v>285</v>
-      </c>
-      <c r="F49" t="s">
+    <row r="55" spans="1:16">
+      <c r="A55" s="7"/>
+      <c r="B55" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="1:16">
+      <c r="A57" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E57" t="s">
+        <v>196</v>
+      </c>
+      <c r="F57" t="s">
         <v>54</v>
       </c>
-      <c r="G49" t="s">
-        <v>11</v>
-      </c>
-      <c r="H49" t="s">
-        <v>75</v>
-      </c>
-      <c r="I49" t="s">
+      <c r="G57" t="s">
+        <v>38</v>
+      </c>
+      <c r="H57" t="s">
+        <v>25</v>
+      </c>
+      <c r="I57" t="s">
         <v>9</v>
       </c>
-      <c r="J49" t="s">
-        <v>31</v>
-      </c>
-      <c r="K49" t="s">
-        <v>27</v>
-      </c>
-      <c r="L49">
-        <v>2014</v>
-      </c>
-      <c r="M49" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N49" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O49" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E50" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="E52" t="s">
-        <v>192</v>
-      </c>
-      <c r="F52" t="s">
-        <v>54</v>
-      </c>
-      <c r="G52" t="s">
-        <v>21</v>
-      </c>
-      <c r="H52" t="s">
-        <v>25</v>
-      </c>
-      <c r="I52" t="s">
-        <v>9</v>
-      </c>
-      <c r="J52" t="s">
-        <v>57</v>
-      </c>
-      <c r="K52" t="s">
+      <c r="J57" t="s">
+        <v>39</v>
+      </c>
+      <c r="K57" t="s">
         <v>20</v>
       </c>
-      <c r="L52">
-        <v>2013</v>
-      </c>
-      <c r="M52" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N52" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="3"/>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>56</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="E55" t="s">
-        <v>190</v>
-      </c>
-      <c r="F55" t="s">
-        <v>54</v>
-      </c>
-      <c r="G55" t="s">
-        <v>21</v>
-      </c>
-      <c r="H55" t="s">
-        <v>25</v>
-      </c>
-      <c r="I55" t="s">
-        <v>9</v>
-      </c>
-      <c r="J55" t="s">
-        <v>51</v>
-      </c>
-      <c r="K55" t="s">
-        <v>20</v>
-      </c>
-      <c r="L55">
-        <v>2013</v>
-      </c>
-      <c r="M55" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N55" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="3"/>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>58</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>183</v>
+      <c r="L57">
+        <v>2009</v>
+      </c>
+      <c r="M57" t="s">
+        <v>298</v>
+      </c>
+      <c r="N57" t="s">
+        <v>59</v>
+      </c>
+      <c r="O57" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
+      <c r="A58" s="7"/>
+      <c r="B58" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>151</v>
       </c>
       <c r="E58" t="s">
-        <v>204</v>
-      </c>
-      <c r="F58" t="s">
-        <v>54</v>
-      </c>
-      <c r="G58" t="s">
-        <v>38</v>
-      </c>
-      <c r="H58" t="s">
-        <v>25</v>
-      </c>
-      <c r="I58" t="s">
-        <v>9</v>
-      </c>
-      <c r="J58" t="s">
-        <v>39</v>
-      </c>
-      <c r="K58" t="s">
-        <v>20</v>
-      </c>
-      <c r="L58">
-        <v>2009</v>
-      </c>
-      <c r="M58" t="s">
-        <v>59</v>
-      </c>
-      <c r="N58" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C59" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="O58" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="D59" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="E59" t="s">
-        <v>203</v>
-      </c>
-      <c r="N59" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:16">
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="O59" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
-      <c r="N60" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O60" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
-      <c r="N61" s="6" t="s">
+      <c r="O61" s="6"/>
+    </row>
+    <row r="62" spans="1:16">
+      <c r="A62" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="N62" s="6"/>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>60</v>
-      </c>
-      <c r="B63" t="s">
-        <v>172</v>
-      </c>
-      <c r="C63" t="s">
-        <v>212</v>
-      </c>
-      <c r="D63" t="s">
-        <v>213</v>
-      </c>
-      <c r="E63" t="s">
-        <v>202</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="C62" t="s">
+        <v>204</v>
+      </c>
+      <c r="D62" t="s">
+        <v>205</v>
+      </c>
+      <c r="E62" t="s">
+        <v>194</v>
+      </c>
+      <c r="F62" t="s">
         <v>54</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G62" t="s">
         <v>38</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H62" t="s">
         <v>25</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I62" t="s">
         <v>9</v>
       </c>
-      <c r="J63" t="s">
+      <c r="J62" t="s">
         <v>43</v>
       </c>
-      <c r="K63" t="s">
+      <c r="K62" t="s">
         <v>27</v>
       </c>
-      <c r="L63" t="s">
+      <c r="L62" t="s">
         <v>42</v>
       </c>
-      <c r="M63" s="1" t="s">
+      <c r="M62" t="s">
+        <v>298</v>
+      </c>
+      <c r="N62" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N63" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="O63" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="7"/>
-      <c r="B64" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+      <c r="O62" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="P62" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
+      <c r="A63" s="7"/>
+      <c r="B63" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" s="2" customFormat="1">
+      <c r="A64" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="E64" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="F64" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G64" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H65" s="2" t="s">
+      <c r="H64" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I65" s="2" t="s">
+      <c r="I64" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J65" s="2" t="s">
+      <c r="J64" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K65" s="2" t="s">
+      <c r="K64" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L65" s="2" t="s">
+      <c r="L64" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M65" s="2" t="s">
+      <c r="N64" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N65" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="O65" s="2" t="s">
+      <c r="O64" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="P64" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="65" spans="1:16">
+      <c r="A65" t="s">
         <v>62</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B65" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="F65" t="s">
+        <v>61</v>
+      </c>
+      <c r="G65" t="s">
+        <v>11</v>
+      </c>
+      <c r="H65" t="s">
+        <v>75</v>
+      </c>
+      <c r="I65" t="s">
+        <v>9</v>
+      </c>
+      <c r="J65" t="s">
+        <v>228</v>
+      </c>
+      <c r="K65" t="s">
+        <v>20</v>
+      </c>
+      <c r="L65">
+        <v>2000</v>
+      </c>
+      <c r="M65" t="s">
         <v>298</v>
       </c>
-      <c r="C66" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="D66" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="E66" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="F66" t="s">
-        <v>61</v>
-      </c>
-      <c r="G66" t="s">
-        <v>11</v>
-      </c>
-      <c r="H66" t="s">
-        <v>75</v>
-      </c>
-      <c r="I66" t="s">
-        <v>9</v>
-      </c>
-      <c r="J66" t="s">
-        <v>236</v>
-      </c>
-      <c r="K66" t="s">
-        <v>20</v>
-      </c>
-      <c r="L66">
-        <v>2000</v>
-      </c>
-      <c r="M66" s="1" t="s">
+      <c r="N65" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N66" s="6" t="s">
+      <c r="O65" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="O66" s="4"/>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
-      <c r="B67" s="9" t="s">
+      <c r="P65" s="4"/>
+    </row>
+    <row r="66" spans="1:16">
+      <c r="A66" s="7"/>
+      <c r="B66" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="C66" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D67" s="9" t="s">
+      <c r="D66" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="N67" s="6" t="s">
+      <c r="O66" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16">
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="O67" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
-      <c r="N68" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="N69" s="6"/>
-    </row>
-    <row r="70" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+      <c r="O68" s="6"/>
+    </row>
+    <row r="69" spans="1:16" s="2" customFormat="1">
+      <c r="A69" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="E69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="F69" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="G69" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="H69" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I70" s="2" t="s">
+      <c r="I69" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J70" s="2" t="s">
+      <c r="J69" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K70" s="2" t="s">
+      <c r="K69" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L70" s="2" t="s">
+      <c r="L69" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M70" s="2" t="s">
+      <c r="N69" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N70" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="O70" s="2" t="s">
+      <c r="O69" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="P69" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="70" spans="1:16">
+      <c r="A70" t="s">
         <v>64</v>
       </c>
-      <c r="B71" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>287</v>
+      <c r="B70" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="E70" t="s">
+        <v>279</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G70" t="s">
+        <v>11</v>
+      </c>
+      <c r="H70" t="s">
+        <v>75</v>
+      </c>
+      <c r="I70" t="s">
+        <v>9</v>
+      </c>
+      <c r="J70" t="s">
+        <v>228</v>
+      </c>
+      <c r="K70" t="s">
+        <v>20</v>
+      </c>
+      <c r="L70">
+        <v>2000</v>
+      </c>
+      <c r="M70" t="s">
+        <v>298</v>
+      </c>
+      <c r="N70" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O70" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16">
+      <c r="A71" s="7"/>
+      <c r="B71" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="E71" t="s">
-        <v>288</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G71" t="s">
-        <v>11</v>
-      </c>
-      <c r="H71" t="s">
-        <v>75</v>
-      </c>
-      <c r="I71" t="s">
-        <v>9</v>
-      </c>
-      <c r="J71" t="s">
-        <v>236</v>
-      </c>
-      <c r="K71" t="s">
-        <v>20</v>
-      </c>
-      <c r="L71">
-        <v>2000</v>
-      </c>
-      <c r="M71" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N71" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A72" s="7"/>
-      <c r="B72" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E72" t="s">
-        <v>209</v>
-      </c>
-      <c r="N72" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="O71" s="6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16">
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="O72" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16">
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
-      <c r="N73" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="N74" s="6"/>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="O73" s="6"/>
+    </row>
+    <row r="74" spans="1:16">
+      <c r="A74" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B75" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="E75" t="s">
-        <v>291</v>
-      </c>
-      <c r="F75" s="1" t="s">
+      <c r="B74" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="E74" t="s">
+        <v>282</v>
+      </c>
+      <c r="F74" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G75" t="s">
+      <c r="G74" t="s">
         <v>11</v>
       </c>
-      <c r="H75" t="s">
+      <c r="H74" t="s">
         <v>76</v>
       </c>
-      <c r="I75" t="s">
+      <c r="I74" t="s">
         <v>9</v>
       </c>
-      <c r="J75" t="s">
+      <c r="J74" t="s">
         <v>67</v>
       </c>
-      <c r="K75" t="s">
+      <c r="K74" t="s">
         <v>20</v>
       </c>
-      <c r="L75">
+      <c r="L74">
         <v>2013</v>
       </c>
-      <c r="M75" s="1" t="s">
+      <c r="M74" t="s">
+        <v>298</v>
+      </c>
+      <c r="N74" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N75" s="6" t="s">
+      <c r="O74" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="O75" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A76" s="7"/>
-      <c r="B76" s="9" t="s">
+      <c r="P74" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16">
+      <c r="A75" s="7"/>
+      <c r="B75" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="C75" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D76" s="9" t="s">
+      <c r="D75" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E76" s="8" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+      <c r="E75" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" s="2" customFormat="1">
+      <c r="A76" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="E76" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="F76" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="G76" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H77" s="2" t="s">
+      <c r="H76" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I77" s="2" t="s">
+      <c r="I76" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J77" s="2" t="s">
+      <c r="J76" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K77" s="2" t="s">
+      <c r="K76" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L77" s="2" t="s">
+      <c r="L76" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M77" s="2" t="s">
+      <c r="N76" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N77" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="O77" s="2" t="s">
+      <c r="O76" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="P76" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    <row r="77" spans="1:16">
+      <c r="A77" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B78" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="E78" t="s">
-        <v>257</v>
-      </c>
-      <c r="F78" s="1" t="s">
+      <c r="B77" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="E77" t="s">
+        <v>248</v>
+      </c>
+      <c r="F77" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G77" t="s">
         <v>21</v>
       </c>
-      <c r="H78" t="s">
+      <c r="H77" t="s">
         <v>25</v>
       </c>
-      <c r="I78" t="s">
+      <c r="I77" t="s">
         <v>9</v>
       </c>
-      <c r="J78" t="s">
+      <c r="J77" t="s">
         <v>19</v>
       </c>
-      <c r="K78" t="s">
+      <c r="K77" t="s">
         <v>20</v>
       </c>
-      <c r="L78" t="s">
+      <c r="L77" t="s">
         <v>28</v>
       </c>
-      <c r="M78" s="1" t="s">
+      <c r="M77" t="s">
+        <v>298</v>
+      </c>
+      <c r="N77" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="N78" s="6" t="s">
+      <c r="O77" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A79" s="7"/>
-      <c r="B79" s="9" t="s">
+    <row r="78" spans="1:16">
+      <c r="A78" s="7"/>
+      <c r="B78" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C79" s="9" t="s">
+      <c r="C78" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="D79" s="9" t="s">
+      <c r="D78" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E79" s="9" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
+      <c r="E78" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" s="2" customFormat="1">
+      <c r="A79" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C79" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="F79" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G80" s="2" t="s">
+      <c r="G79" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H80" s="2" t="s">
+      <c r="H79" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I80" s="2" t="s">
+      <c r="I79" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J80" s="2" t="s">
+      <c r="J79" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K80" s="2" t="s">
+      <c r="K79" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L80" s="2" t="s">
+      <c r="L79" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M80" s="2" t="s">
+      <c r="N79" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N80" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="O80" s="2" t="s">
+      <c r="O79" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="P79" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="80" spans="1:16">
+      <c r="A80" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B81" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="E81" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="F81" s="1" t="s">
+      <c r="B80" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="E80" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="F80" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G80" t="s">
         <v>21</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H80" t="s">
         <v>25</v>
       </c>
-      <c r="I81" t="s">
+      <c r="I80" t="s">
         <v>9</v>
       </c>
-      <c r="J81" t="s">
+      <c r="J80" t="s">
         <v>72</v>
       </c>
-      <c r="K81" t="s">
+      <c r="K80" t="s">
         <v>27</v>
       </c>
-      <c r="L81" t="s">
+      <c r="L80" t="s">
         <v>28</v>
       </c>
-      <c r="M81" s="1" t="s">
+      <c r="M80" t="s">
+        <v>298</v>
+      </c>
+      <c r="N80" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="N81" s="6" t="s">
+      <c r="O80" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A82" s="7"/>
-      <c r="B82" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="D82" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>293</v>
-      </c>
-      <c r="F84" t="s">
-        <v>294</v>
-      </c>
-      <c r="G84" t="s">
+    <row r="81" spans="1:14">
+      <c r="A81" s="7"/>
+      <c r="B81" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14">
+      <c r="A83" t="s">
+        <v>284</v>
+      </c>
+      <c r="F83" t="s">
+        <v>285</v>
+      </c>
+      <c r="G83" t="s">
         <v>11</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H83" t="s">
         <v>75</v>
       </c>
-      <c r="J84" t="s">
-        <v>295</v>
-      </c>
-      <c r="K84" t="s">
+      <c r="J83" t="s">
+        <v>286</v>
+      </c>
+      <c r="K83" t="s">
         <v>20</v>
       </c>
-      <c r="L84">
+      <c r="L83">
         <v>2000</v>
       </c>
-      <c r="M84" t="s">
-        <v>296</v>
+      <c r="M83" t="s">
+        <v>298</v>
+      </c>
+      <c r="N83" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1"/>
-    <hyperlink ref="N75" r:id="rId2"/>
-    <hyperlink ref="N66" r:id="rId3"/>
-    <hyperlink ref="N49" r:id="rId4"/>
-    <hyperlink ref="N71" r:id="rId5"/>
-    <hyperlink ref="N33" r:id="rId6"/>
-    <hyperlink ref="N36" r:id="rId7"/>
-    <hyperlink ref="N14" r:id="rId8"/>
-    <hyperlink ref="N17" r:id="rId9"/>
-    <hyperlink ref="N18" r:id="rId10"/>
-    <hyperlink ref="N37" r:id="rId11"/>
-    <hyperlink ref="N67" r:id="rId12"/>
-    <hyperlink ref="N72" r:id="rId13"/>
-    <hyperlink ref="N68" r:id="rId14"/>
-    <hyperlink ref="N73" r:id="rId15"/>
-    <hyperlink ref="N5" r:id="rId16"/>
-    <hyperlink ref="N8" r:id="rId17"/>
-    <hyperlink ref="N11" r:id="rId18"/>
-    <hyperlink ref="N20" r:id="rId19"/>
-    <hyperlink ref="N39" r:id="rId20"/>
-    <hyperlink ref="N43" r:id="rId21"/>
-    <hyperlink ref="N46" r:id="rId22"/>
-    <hyperlink ref="N52" r:id="rId23"/>
-    <hyperlink ref="N55" r:id="rId24"/>
-    <hyperlink ref="N78" r:id="rId25"/>
-    <hyperlink ref="N81" r:id="rId26"/>
-    <hyperlink ref="N40" r:id="rId27"/>
-    <hyperlink ref="N41" r:id="rId28"/>
-    <hyperlink ref="N6" r:id="rId29"/>
-    <hyperlink ref="N25" r:id="rId30"/>
-    <hyperlink ref="N30" r:id="rId31"/>
-    <hyperlink ref="N58" r:id="rId32"/>
-    <hyperlink ref="N63" r:id="rId33"/>
-    <hyperlink ref="N26" r:id="rId34"/>
-    <hyperlink ref="N59" r:id="rId35"/>
-    <hyperlink ref="N27" r:id="rId36"/>
-    <hyperlink ref="N60" r:id="rId37"/>
-    <hyperlink ref="N28" r:id="rId38"/>
-    <hyperlink ref="N61" r:id="rId39"/>
+    <hyperlink ref="O2" r:id="rId1"/>
+    <hyperlink ref="O74" r:id="rId2"/>
+    <hyperlink ref="O65" r:id="rId3"/>
+    <hyperlink ref="O48" r:id="rId4"/>
+    <hyperlink ref="O70" r:id="rId5"/>
+    <hyperlink ref="O32" r:id="rId6"/>
+    <hyperlink ref="O35" r:id="rId7"/>
+    <hyperlink ref="O13" r:id="rId8"/>
+    <hyperlink ref="O16" r:id="rId9"/>
+    <hyperlink ref="O17" r:id="rId10"/>
+    <hyperlink ref="O36" r:id="rId11"/>
+    <hyperlink ref="O66" r:id="rId12"/>
+    <hyperlink ref="O71" r:id="rId13"/>
+    <hyperlink ref="O67" r:id="rId14"/>
+    <hyperlink ref="O72" r:id="rId15"/>
+    <hyperlink ref="O5" r:id="rId16"/>
+    <hyperlink ref="O8" r:id="rId17"/>
+    <hyperlink ref="O10" r:id="rId18"/>
+    <hyperlink ref="O19" r:id="rId19"/>
+    <hyperlink ref="O38" r:id="rId20"/>
+    <hyperlink ref="O42" r:id="rId21"/>
+    <hyperlink ref="O45" r:id="rId22"/>
+    <hyperlink ref="O51" r:id="rId23"/>
+    <hyperlink ref="O54" r:id="rId24"/>
+    <hyperlink ref="O77" r:id="rId25"/>
+    <hyperlink ref="O80" r:id="rId26"/>
+    <hyperlink ref="O39" r:id="rId27"/>
+    <hyperlink ref="O40" r:id="rId28"/>
+    <hyperlink ref="O6" r:id="rId29"/>
+    <hyperlink ref="O24" r:id="rId30"/>
+    <hyperlink ref="O29" r:id="rId31"/>
+    <hyperlink ref="O57" r:id="rId32"/>
+    <hyperlink ref="O62" r:id="rId33"/>
+    <hyperlink ref="O25" r:id="rId34"/>
+    <hyperlink ref="O58" r:id="rId35"/>
+    <hyperlink ref="O26" r:id="rId36"/>
+    <hyperlink ref="O59" r:id="rId37"/>
+    <hyperlink ref="O27" r:id="rId38"/>
+    <hyperlink ref="O60" r:id="rId39"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3855,25 +3902,25 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="75.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" s="3" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
[corpus] metadata for stories updated
</commit_message>
<xml_diff>
--- a/corpus/comparable/metadata.xlsx
+++ b/corpus/comparable/metadata.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="299">
   <si>
     <t>Langue</t>
   </si>
@@ -940,15 +940,6 @@
     <t>KLR_SOLME2_Dhana.163</t>
   </si>
   <si>
-    <t>2&amp; that TB can't resolve; otherwise READY (but check against recording)</t>
-  </si>
-  <si>
-    <t>Some &amp; that TB can't resolve, otherwise READY (but check against recording)</t>
-  </si>
-  <si>
-    <t>3&amp; that Toolbox can't resolve; otherwise, ready for archiving (but check against recording)</t>
-  </si>
-  <si>
     <t>Lieu</t>
   </si>
   <si>
@@ -959,6 +950,9 @@
   </si>
   <si>
     <t>Friday 17 April 2015</t>
+  </si>
+  <si>
+    <t>Archived</t>
   </si>
 </sst>
 </file>
@@ -971,7 +965,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1212,7 +1205,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1225,6 +1218,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="171">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -1733,21 +1729,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="2" max="2" width="58.875" customWidth="1"/>
-    <col min="3" max="4" width="34.75" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="58.83203125" customWidth="1"/>
+    <col min="3" max="4" width="34.6640625" customWidth="1"/>
     <col min="5" max="5" width="41.5" customWidth="1"/>
-    <col min="6" max="6" width="24.875" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
     <col min="14" max="14" width="63" customWidth="1"/>
-    <col min="15" max="15" width="85.625" customWidth="1"/>
+    <col min="15" max="15" width="85.6640625" customWidth="1"/>
     <col min="16" max="16" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1789,7 +1785,7 @@
         <v>4</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>5</v>
@@ -1839,7 +1835,7 @@
         <v>2000</v>
       </c>
       <c r="M2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>12</v>
@@ -1847,7 +1843,9 @@
       <c r="O2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P2" s="4"/>
+      <c r="P2" s="10" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="7"/>
@@ -1862,12 +1860,14 @@
       </c>
       <c r="E3" s="9"/>
       <c r="O3" s="6"/>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" spans="1:16">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="O4" s="6"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
@@ -1907,7 +1907,7 @@
         <v>22</v>
       </c>
       <c r="M5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>12</v>
@@ -1915,8 +1915,8 @@
       <c r="O5" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="P5" s="3" t="s">
-        <v>294</v>
+      <c r="P5" s="8" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1929,11 +1929,13 @@
       <c r="O6" s="6" t="s">
         <v>141</v>
       </c>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" spans="1:16">
       <c r="B7" s="3"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
@@ -1973,7 +1975,7 @@
         <v>22</v>
       </c>
       <c r="M8" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>12</v>
@@ -1981,12 +1983,13 @@
       <c r="O8" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="P8" s="3" t="s">
-        <v>295</v>
+      <c r="P8" s="8" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="B9" s="3"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
@@ -2026,7 +2029,7 @@
         <v>28</v>
       </c>
       <c r="M10" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>12</v>
@@ -2034,8 +2037,8 @@
       <c r="O10" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="P10" s="1" t="s">
-        <v>296</v>
+      <c r="P10" s="8" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -2138,7 +2141,7 @@
         <v>2014</v>
       </c>
       <c r="M13" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>12</v>
@@ -2205,7 +2208,7 @@
         <v>2009</v>
       </c>
       <c r="M16" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>33</v>
@@ -2276,7 +2279,7 @@
         <v>42</v>
       </c>
       <c r="M19" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N19" t="s">
         <v>12</v>
@@ -2374,7 +2377,7 @@
         <v>2004</v>
       </c>
       <c r="M24" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>40</v>
@@ -2461,7 +2464,7 @@
         <v>42</v>
       </c>
       <c r="M29" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>12</v>
@@ -2573,7 +2576,7 @@
         <v>2014</v>
       </c>
       <c r="M32" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>12</v>
@@ -2643,7 +2646,7 @@
         <v>2009</v>
       </c>
       <c r="M35" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N35" s="1" t="s">
         <v>47</v>
@@ -2717,7 +2720,7 @@
         <v>2011</v>
       </c>
       <c r="M38" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>232</v>
@@ -2795,7 +2798,7 @@
         <v>2013</v>
       </c>
       <c r="M42" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="N42" s="1" t="s">
         <v>12</v>
@@ -2860,7 +2863,7 @@
         <v>2013</v>
       </c>
       <c r="M45" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N45" s="1" t="s">
         <v>12</v>
@@ -2969,7 +2972,7 @@
         <v>2014</v>
       </c>
       <c r="M48" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N48" s="1" t="s">
         <v>12</v>
@@ -3039,7 +3042,7 @@
         <v>2013</v>
       </c>
       <c r="M51" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N51" s="1" t="s">
         <v>12</v>
@@ -3104,7 +3107,7 @@
         <v>2013</v>
       </c>
       <c r="M54" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N54" s="1" t="s">
         <v>12</v>
@@ -3169,7 +3172,7 @@
         <v>2009</v>
       </c>
       <c r="M57" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N57" t="s">
         <v>59</v>
@@ -3256,7 +3259,7 @@
         <v>42</v>
       </c>
       <c r="M62" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N62" s="1" t="s">
         <v>12</v>
@@ -3368,7 +3371,7 @@
         <v>2000</v>
       </c>
       <c r="M65" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N65" s="1" t="s">
         <v>12</v>
@@ -3492,7 +3495,7 @@
         <v>2000</v>
       </c>
       <c r="M70" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N70" s="1" t="s">
         <v>65</v>
@@ -3571,7 +3574,7 @@
         <v>2013</v>
       </c>
       <c r="M74" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N74" s="1" t="s">
         <v>12</v>
@@ -3683,7 +3686,7 @@
         <v>28</v>
       </c>
       <c r="M77" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N77" s="1" t="s">
         <v>69</v>
@@ -3792,7 +3795,7 @@
         <v>28</v>
       </c>
       <c r="M80" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N80" s="1" t="s">
         <v>69</v>
@@ -3839,7 +3842,7 @@
         <v>2000</v>
       </c>
       <c r="M83" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N83" t="s">
         <v>287</v>
@@ -3905,9 +3908,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="75.125" customWidth="1"/>
+    <col min="1" max="1" width="75.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -3917,7 +3920,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:1">

</xml_diff>

<commit_message>
changes to comparable corpus metadata--story inventory: one added
</commit_message>
<xml_diff>
--- a/corpus/comparable/metadata.xlsx
+++ b/corpus/comparable/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25620" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="302">
   <si>
     <t>Langue</t>
   </si>
@@ -953,6 +953,15 @@
   </si>
   <si>
     <t>Archived</t>
+  </si>
+  <si>
+    <t>Vulture</t>
+  </si>
+  <si>
+    <t>TDH-Mukli_Vulture_Chandrakala</t>
+  </si>
+  <si>
+    <t>Paris</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1041,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="171">
+  <cellStyleXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1204,8 +1213,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1221,8 +1231,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="171">
+  <cellStyles count="172">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -1393,6 +1404,7 @@
     <cellStyle name="Lien hypertexte visité" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="169" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="171" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1727,10 +1739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1863,149 +1875,146 @@
       <c r="P3" s="8"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
       <c r="O4" s="6"/>
       <c r="P4" s="8"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" t="s">
-        <v>23</v>
+      <c r="A5" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C5" t="s">
-        <v>233</v>
-      </c>
-      <c r="D5" t="s">
-        <v>283</v>
-      </c>
-      <c r="E5" t="s">
-        <v>239</v>
+        <v>300</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="8" t="s">
+        <v>300</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="I5" t="s">
         <v>9</v>
       </c>
       <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="11">
+        <v>42248</v>
+      </c>
+      <c r="M5" t="s">
+        <v>301</v>
+      </c>
+      <c r="N5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" s="6"/>
+      <c r="P5" s="8"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="8"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D7" t="s">
+        <v>283</v>
+      </c>
+      <c r="E7" t="s">
+        <v>239</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" t="s">
         <v>19</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K7" t="s">
         <v>20</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L7" t="s">
         <v>22</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M7" t="s">
         <v>295</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="O7" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P7" s="8" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="7"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="6" t="s">
+    <row r="8" spans="1:16">
+      <c r="A8" s="7"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="P6" s="8"/>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="B7" s="3"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="8"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="C8" t="s">
-        <v>234</v>
-      </c>
-      <c r="D8" t="s">
-        <v>293</v>
-      </c>
-      <c r="E8" t="s">
-        <v>238</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" t="s">
-        <v>295</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="P8" s="8" t="s">
-        <v>298</v>
-      </c>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" spans="1:16">
       <c r="B9" s="3"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
       <c r="P9" s="8"/>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D10" t="s">
-        <v>236</v>
+        <v>293</v>
       </c>
       <c r="E10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>
@@ -2020,13 +2029,13 @@
         <v>9</v>
       </c>
       <c r="J10" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="K10" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="M10" t="s">
         <v>295</v>
@@ -2042,1853 +2051,1907 @@
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="7"/>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="3"/>
+      <c r="P11" s="8"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C12" t="s">
+        <v>235</v>
+      </c>
+      <c r="D12" t="s">
+        <v>236</v>
+      </c>
+      <c r="E12" t="s">
+        <v>237</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" t="s">
+        <v>295</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="7"/>
+      <c r="B13" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D13" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E13" s="9" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="2" customFormat="1">
-      <c r="A12" s="2" t="s">
+    <row r="14" spans="1:16" s="2" customFormat="1">
+      <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="N14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="O14" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="P14" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
-      <c r="A13" t="s">
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B15" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C15" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D15" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E15" t="s">
         <v>264</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F15" t="s">
         <v>29</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G15" t="s">
         <v>11</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H15" t="s">
         <v>75</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I15" t="s">
         <v>9</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J15" t="s">
         <v>31</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K15" t="s">
         <v>27</v>
       </c>
-      <c r="L13">
+      <c r="L15">
         <v>2014</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M15" t="s">
         <v>295</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O13" s="6" t="s">
+      <c r="O15" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="7"/>
-      <c r="B14" s="9" t="s">
+    <row r="16" spans="1:16">
+      <c r="A16" s="7"/>
+      <c r="B16" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C16" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E16" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" t="s">
+    <row r="17" spans="1:16">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B18" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C18" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E18" t="s">
         <v>267</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F18" t="s">
         <v>29</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G18" t="s">
         <v>11</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H18" t="s">
         <v>76</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I18" t="s">
         <v>9</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J18" t="s">
         <v>32</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K18" t="s">
         <v>20</v>
       </c>
-      <c r="L16">
+      <c r="L18">
         <v>2009</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M18" t="s">
         <v>295</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O16" s="6" t="s">
+      <c r="O18" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="7"/>
-      <c r="B17" s="9" t="s">
+    <row r="19" spans="1:16">
+      <c r="A19" s="7"/>
+      <c r="B19" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C19" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D19" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E19" t="s">
         <v>198</v>
       </c>
-      <c r="O17" s="6" t="s">
+      <c r="O19" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="O18" s="6"/>
-    </row>
-    <row r="19" spans="1:16">
-      <c r="A19" t="s">
+    <row r="20" spans="1:16">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="O20" s="6"/>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" t="s">
         <v>34</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>167</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>168</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D21" t="s">
         <v>169</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E21" t="s">
         <v>188</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F21" t="s">
         <v>29</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G21" t="s">
         <v>21</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H21" t="s">
         <v>25</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I21" t="s">
         <v>9</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J21" t="s">
         <v>19</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K21" t="s">
         <v>20</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L21" t="s">
         <v>42</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M21" t="s">
         <v>295</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N21" t="s">
         <v>12</v>
       </c>
-      <c r="O19" s="6" t="s">
+      <c r="O21" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="7"/>
-      <c r="B20" s="9" t="s">
+    <row r="22" spans="1:16">
+      <c r="A22" s="7"/>
+      <c r="B22" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C22" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D22" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E22" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:16">
-      <c r="A22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="F22" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22" t="s">
-        <v>35</v>
-      </c>
-      <c r="O22" s="6"/>
-      <c r="P22" s="3" t="s">
-        <v>36</v>
-      </c>
+    <row r="23" spans="1:16">
+      <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:16">
       <c r="A24" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="C24" t="s">
-        <v>252</v>
-      </c>
-      <c r="D24" t="s">
-        <v>253</v>
-      </c>
-      <c r="E24" t="s">
-        <v>254</v>
+        <v>217</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>256</v>
       </c>
       <c r="F24" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="G24" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="H24" t="s">
         <v>25</v>
       </c>
       <c r="I24" t="s">
+        <v>35</v>
+      </c>
+      <c r="O24" s="6"/>
+      <c r="P24" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C26" t="s">
+        <v>252</v>
+      </c>
+      <c r="D26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E26" t="s">
+        <v>254</v>
+      </c>
+      <c r="F26" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" t="s">
         <v>9</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J26" t="s">
         <v>39</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K26" t="s">
         <v>20</v>
       </c>
-      <c r="L24">
+      <c r="L26">
         <v>2004</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M26" t="s">
         <v>295</v>
       </c>
-      <c r="N24" s="1" t="s">
+      <c r="N26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O24" s="6" t="s">
+      <c r="O26" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="7"/>
-      <c r="B25" s="9" t="s">
+    <row r="27" spans="1:16">
+      <c r="A27" s="7"/>
+      <c r="B27" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D27" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E27" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="O25" s="6" t="s">
+      <c r="O27" s="6" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="O26" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="O27" s="6" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:16">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="O28" s="6"/>
+      <c r="O28" s="6" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" t="s">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="O29" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="O30" s="6"/>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B31" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C31" t="s">
         <v>257</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D31" t="s">
         <v>258</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E31" t="s">
         <v>259</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F31" t="s">
         <v>53</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G31" t="s">
         <v>38</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H31" t="s">
         <v>25</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I31" t="s">
         <v>9</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J31" t="s">
         <v>43</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K31" t="s">
         <v>27</v>
       </c>
-      <c r="L29" t="s">
+      <c r="L31" t="s">
         <v>42</v>
       </c>
-      <c r="M29" t="s">
+      <c r="M31" t="s">
         <v>295</v>
       </c>
-      <c r="N29" s="1" t="s">
+      <c r="N31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O29" s="6" t="s">
+      <c r="O31" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="P29" s="3" t="s">
+      <c r="P31" s="3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
-      <c r="A30" s="7"/>
-      <c r="B30" s="9" t="s">
+    <row r="32" spans="1:16">
+      <c r="A32" s="7"/>
+      <c r="B32" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C32" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D32" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E32" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="2" customFormat="1">
-      <c r="A31" s="2" t="s">
+    <row r="33" spans="1:16" s="2" customFormat="1">
+      <c r="A33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="J33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="K33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L31" s="2" t="s">
+      <c r="L33" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N31" s="2" t="s">
+      <c r="N33" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O31" s="2" t="s">
+      <c r="O33" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="P31" s="2" t="s">
+      <c r="P33" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
-      <c r="A32" t="s">
+    <row r="34" spans="1:16">
+      <c r="A34" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B34" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C34" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D34" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E34" t="s">
         <v>270</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F34" t="s">
         <v>44</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G34" t="s">
         <v>11</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H34" t="s">
         <v>75</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I34" t="s">
         <v>9</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J34" t="s">
         <v>31</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K34" t="s">
         <v>27</v>
       </c>
-      <c r="L32">
+      <c r="L34">
         <v>2014</v>
       </c>
-      <c r="M32" t="s">
+      <c r="M34" t="s">
         <v>295</v>
       </c>
-      <c r="N32" s="1" t="s">
+      <c r="N34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O32" s="6" t="s">
+      <c r="O34" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="P32" s="3" t="s">
+      <c r="P34" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
-      <c r="A33" s="7"/>
-      <c r="B33" s="9" t="s">
+    <row r="35" spans="1:16">
+      <c r="A35" s="7"/>
+      <c r="B35" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C35" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D35" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E35" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:16">
-      <c r="A35" t="s">
+    <row r="36" spans="1:16">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B37" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C37" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D37" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E37" t="s">
         <v>273</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F37" t="s">
         <v>44</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G37" t="s">
         <v>11</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H37" t="s">
         <v>76</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I37" t="s">
         <v>9</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J37" t="s">
         <v>32</v>
       </c>
-      <c r="K35" t="s">
+      <c r="K37" t="s">
         <v>20</v>
       </c>
-      <c r="L35">
+      <c r="L37">
         <v>2009</v>
       </c>
-      <c r="M35" t="s">
+      <c r="M37" t="s">
         <v>295</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="N37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="O35" s="6" t="s">
+      <c r="O37" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="P35" s="3" t="s">
+      <c r="P37" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
-      <c r="A36" s="7"/>
-      <c r="B36" s="9" t="s">
+    <row r="38" spans="1:16">
+      <c r="A38" s="7"/>
+      <c r="B38" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C38" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D38" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E38" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="O36" s="6" t="s">
+      <c r="O38" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="O37" s="6"/>
-    </row>
-    <row r="38" spans="1:16">
-      <c r="A38" t="s">
+    <row r="39" spans="1:16">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="O39" s="6"/>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B40" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C40" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D40" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F40" t="s">
         <v>44</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G40" t="s">
         <v>21</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H40" t="s">
         <v>25</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I40" t="s">
         <v>9</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J40" t="s">
         <v>19</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K40" t="s">
         <v>20</v>
       </c>
-      <c r="L38">
+      <c r="L40">
         <v>2011</v>
       </c>
-      <c r="M38" t="s">
+      <c r="M40" t="s">
         <v>295</v>
       </c>
-      <c r="N38" s="1" t="s">
+      <c r="N40" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="O38" s="6" t="s">
+      <c r="O40" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
-      <c r="A39" s="7"/>
-      <c r="B39" s="9" t="s">
+    <row r="41" spans="1:16">
+      <c r="A41" s="7"/>
+      <c r="B41" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C41" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D41" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E41" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="O39" s="6" t="s">
+      <c r="O41" s="6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="O40" s="6" t="s">
+    <row r="42" spans="1:16">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="O42" s="6" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:16">
-      <c r="A42" t="s">
+    <row r="43" spans="1:16">
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B44" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C44" t="s">
         <v>240</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D44" t="s">
         <v>241</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E44" t="s">
         <v>242</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F44" t="s">
         <v>44</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G44" t="s">
         <v>21</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H44" t="s">
         <v>25</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I44" t="s">
         <v>9</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J44" t="s">
         <v>49</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K44" t="s">
         <v>20</v>
       </c>
-      <c r="L42">
+      <c r="L44">
         <v>2013</v>
       </c>
-      <c r="M42" t="s">
+      <c r="M44" t="s">
         <v>296</v>
       </c>
-      <c r="N42" s="1" t="s">
+      <c r="N44" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O42" s="6" t="s">
+      <c r="O44" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
-      <c r="A43" s="7"/>
-      <c r="B43" s="9" t="s">
+    <row r="45" spans="1:16">
+      <c r="A45" s="7"/>
+      <c r="B45" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C45" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D45" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E45" s="9" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="1:16">
-      <c r="A45" t="s">
+    <row r="46" spans="1:16">
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B47" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C47" t="s">
         <v>243</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D47" t="s">
         <v>244</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E47" t="s">
         <v>245</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F47" t="s">
         <v>44</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G47" t="s">
         <v>21</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H47" t="s">
         <v>25</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I47" t="s">
         <v>9</v>
       </c>
-      <c r="J45" t="s">
+      <c r="J47" t="s">
         <v>51</v>
       </c>
-      <c r="K45" t="s">
+      <c r="K47" t="s">
         <v>20</v>
       </c>
-      <c r="L45">
+      <c r="L47">
         <v>2013</v>
       </c>
-      <c r="M45" t="s">
+      <c r="M47" t="s">
         <v>295</v>
       </c>
-      <c r="N45" s="1" t="s">
+      <c r="N47" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O45" s="6" t="s">
+      <c r="O47" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
-      <c r="A46" s="7"/>
-      <c r="B46" s="9" t="s">
+    <row r="48" spans="1:16">
+      <c r="A48" s="7"/>
+      <c r="B48" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C48" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D48" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E48" s="9" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="2" customFormat="1">
-      <c r="A47" s="2" t="s">
+    <row r="49" spans="1:16" s="2" customFormat="1">
+      <c r="A49" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I47" s="2" t="s">
+      <c r="I49" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J47" s="2" t="s">
+      <c r="J49" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K47" s="2" t="s">
+      <c r="K49" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L47" s="2" t="s">
+      <c r="L49" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N47" s="2" t="s">
+      <c r="N49" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O47" s="2" t="s">
+      <c r="O49" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="P47" s="2" t="s">
+      <c r="P49" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
-      <c r="A48" t="s">
+    <row r="50" spans="1:16">
+      <c r="A50" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B50" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C50" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D50" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E50" t="s">
         <v>276</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F50" t="s">
         <v>54</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G50" t="s">
         <v>11</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H50" t="s">
         <v>75</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I50" t="s">
         <v>9</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J50" t="s">
         <v>31</v>
       </c>
-      <c r="K48" t="s">
+      <c r="K50" t="s">
         <v>27</v>
       </c>
-      <c r="L48">
+      <c r="L50">
         <v>2014</v>
       </c>
-      <c r="M48" t="s">
+      <c r="M50" t="s">
         <v>295</v>
       </c>
-      <c r="N48" s="1" t="s">
+      <c r="N50" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O48" s="6" t="s">
+      <c r="O50" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="P48" s="3" t="s">
+      <c r="P50" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
-      <c r="A49" s="7"/>
-      <c r="B49" s="9" t="s">
+    <row r="51" spans="1:16">
+      <c r="A51" s="7"/>
+      <c r="B51" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C51" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D49" s="9" t="s">
+      <c r="D51" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E51" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:16">
-      <c r="A51" t="s">
+    <row r="52" spans="1:16">
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="A53" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B53" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C53" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D53" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E53" t="s">
         <v>186</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F53" t="s">
         <v>54</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G53" t="s">
         <v>21</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H53" t="s">
         <v>25</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I53" t="s">
         <v>9</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J53" t="s">
         <v>57</v>
       </c>
-      <c r="K51" t="s">
+      <c r="K53" t="s">
         <v>20</v>
       </c>
-      <c r="L51">
+      <c r="L53">
         <v>2013</v>
       </c>
-      <c r="M51" t="s">
+      <c r="M53" t="s">
         <v>295</v>
       </c>
-      <c r="N51" s="1" t="s">
+      <c r="N53" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O51" s="6" t="s">
+      <c r="O53" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
-      <c r="A52" s="7"/>
-      <c r="B52" s="9" t="s">
+    <row r="54" spans="1:16">
+      <c r="A54" s="7"/>
+      <c r="B54" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C54" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D52" s="9" t="s">
+      <c r="D54" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="E52" s="9" t="s">
+      <c r="E54" s="9" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="1:16">
-      <c r="A54" t="s">
+    <row r="55" spans="1:16">
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="A56" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B56" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C56" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D56" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E56" t="s">
         <v>184</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F56" t="s">
         <v>54</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G56" t="s">
         <v>21</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H56" t="s">
         <v>25</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I56" t="s">
         <v>9</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J56" t="s">
         <v>51</v>
       </c>
-      <c r="K54" t="s">
+      <c r="K56" t="s">
         <v>20</v>
       </c>
-      <c r="L54">
+      <c r="L56">
         <v>2013</v>
       </c>
-      <c r="M54" t="s">
+      <c r="M56" t="s">
         <v>295</v>
       </c>
-      <c r="N54" s="1" t="s">
+      <c r="N56" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O54" s="6" t="s">
+      <c r="O56" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
-      <c r="A55" s="7"/>
-      <c r="B55" s="9" t="s">
+    <row r="57" spans="1:16">
+      <c r="A57" s="7"/>
+      <c r="B57" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C57" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D55" s="9" t="s">
+      <c r="D57" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="E55" s="9" t="s">
+      <c r="E57" s="9" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
-      <c r="B56" s="3"/>
-    </row>
-    <row r="57" spans="1:16">
-      <c r="A57" t="s">
+    <row r="58" spans="1:16">
+      <c r="B58" s="3"/>
+    </row>
+    <row r="59" spans="1:16">
+      <c r="A59" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B59" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C59" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="D59" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E59" t="s">
         <v>196</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F59" t="s">
         <v>54</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G59" t="s">
         <v>38</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H59" t="s">
         <v>25</v>
       </c>
-      <c r="I57" t="s">
+      <c r="I59" t="s">
         <v>9</v>
       </c>
-      <c r="J57" t="s">
+      <c r="J59" t="s">
         <v>39</v>
       </c>
-      <c r="K57" t="s">
+      <c r="K59" t="s">
         <v>20</v>
       </c>
-      <c r="L57">
+      <c r="L59">
         <v>2009</v>
       </c>
-      <c r="M57" t="s">
+      <c r="M59" t="s">
         <v>295</v>
       </c>
-      <c r="N57" t="s">
+      <c r="N59" t="s">
         <v>59</v>
       </c>
-      <c r="O57" s="6" t="s">
+      <c r="O59" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
-      <c r="A58" s="7"/>
-      <c r="B58" s="9" t="s">
+    <row r="60" spans="1:16">
+      <c r="A60" s="7"/>
+      <c r="B60" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C60" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="D58" s="9" t="s">
+      <c r="D60" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E60" t="s">
         <v>195</v>
       </c>
-      <c r="O58" s="6" t="s">
+      <c r="O60" s="6" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16">
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="O59" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16">
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="O60" s="6" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="61" spans="1:16">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
-      <c r="O61" s="6"/>
+      <c r="O61" s="6" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="62" spans="1:16">
-      <c r="A62" t="s">
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="O62" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="O63" s="6"/>
+    </row>
+    <row r="64" spans="1:16">
+      <c r="A64" t="s">
         <v>60</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B64" t="s">
         <v>166</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C64" t="s">
         <v>204</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D64" t="s">
         <v>205</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E64" t="s">
         <v>194</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F64" t="s">
         <v>54</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G64" t="s">
         <v>38</v>
       </c>
-      <c r="H62" t="s">
+      <c r="H64" t="s">
         <v>25</v>
       </c>
-      <c r="I62" t="s">
+      <c r="I64" t="s">
         <v>9</v>
       </c>
-      <c r="J62" t="s">
+      <c r="J64" t="s">
         <v>43</v>
       </c>
-      <c r="K62" t="s">
+      <c r="K64" t="s">
         <v>27</v>
       </c>
-      <c r="L62" t="s">
+      <c r="L64" t="s">
         <v>42</v>
       </c>
-      <c r="M62" t="s">
+      <c r="M64" t="s">
         <v>295</v>
       </c>
-      <c r="N62" s="1" t="s">
+      <c r="N64" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O62" s="6" t="s">
+      <c r="O64" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="P62" s="3" t="s">
+      <c r="P64" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
-      <c r="A63" s="7"/>
-      <c r="B63" s="9" t="s">
+    <row r="65" spans="1:16">
+      <c r="A65" s="7"/>
+      <c r="B65" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C63" s="9" t="s">
+      <c r="C65" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="D63" s="9" t="s">
+      <c r="D65" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="E65" s="8" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="64" spans="1:16" s="2" customFormat="1">
-      <c r="A64" s="2" t="s">
+    <row r="66" spans="1:16" s="2" customFormat="1">
+      <c r="A66" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G66" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H64" s="2" t="s">
+      <c r="H66" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I64" s="2" t="s">
+      <c r="I66" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J64" s="2" t="s">
+      <c r="J66" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K64" s="2" t="s">
+      <c r="K66" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L64" s="2" t="s">
+      <c r="L66" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N64" s="2" t="s">
+      <c r="N66" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O64" s="2" t="s">
+      <c r="O66" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="P64" s="2" t="s">
+      <c r="P66" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
-      <c r="A65" t="s">
+    <row r="67" spans="1:16">
+      <c r="A67" t="s">
         <v>62</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B67" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C67" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="D65" s="8" t="s">
+      <c r="D67" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="E65" s="8" t="s">
+      <c r="E67" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F67" t="s">
         <v>61</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G67" t="s">
         <v>11</v>
       </c>
-      <c r="H65" t="s">
+      <c r="H67" t="s">
         <v>75</v>
       </c>
-      <c r="I65" t="s">
+      <c r="I67" t="s">
         <v>9</v>
       </c>
-      <c r="J65" t="s">
+      <c r="J67" t="s">
         <v>228</v>
       </c>
-      <c r="K65" t="s">
+      <c r="K67" t="s">
         <v>20</v>
       </c>
-      <c r="L65">
+      <c r="L67">
         <v>2000</v>
       </c>
-      <c r="M65" t="s">
+      <c r="M67" t="s">
         <v>295</v>
       </c>
-      <c r="N65" s="1" t="s">
+      <c r="N67" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O65" s="6" t="s">
+      <c r="O67" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="P65" s="4"/>
-    </row>
-    <row r="66" spans="1:16">
-      <c r="A66" s="7"/>
-      <c r="B66" s="9" t="s">
+      <c r="P67" s="4"/>
+    </row>
+    <row r="68" spans="1:16">
+      <c r="A68" s="7"/>
+      <c r="B68" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="C68" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D66" s="9" t="s">
+      <c r="D68" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="O66" s="6" t="s">
+      <c r="O68" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="O67" s="6" t="s">
+    <row r="69" spans="1:16">
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="O69" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="O68" s="6"/>
-    </row>
-    <row r="69" spans="1:16" s="2" customFormat="1">
-      <c r="A69" s="2" t="s">
+    <row r="70" spans="1:16">
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="O70" s="6"/>
+    </row>
+    <row r="71" spans="1:16" s="2" customFormat="1">
+      <c r="A71" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="E71" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H69" s="2" t="s">
+      <c r="H71" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I69" s="2" t="s">
+      <c r="I71" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J69" s="2" t="s">
+      <c r="J71" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K69" s="2" t="s">
+      <c r="K71" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L69" s="2" t="s">
+      <c r="L71" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N69" s="2" t="s">
+      <c r="N71" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O69" s="2" t="s">
+      <c r="O71" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="P69" s="2" t="s">
+      <c r="P71" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
-      <c r="A70" t="s">
+    <row r="72" spans="1:16">
+      <c r="A72" t="s">
         <v>64</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B72" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="C72" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="D72" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E72" t="s">
         <v>279</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="F72" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G72" t="s">
         <v>11</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H72" t="s">
         <v>75</v>
       </c>
-      <c r="I70" t="s">
+      <c r="I72" t="s">
         <v>9</v>
       </c>
-      <c r="J70" t="s">
+      <c r="J72" t="s">
         <v>228</v>
       </c>
-      <c r="K70" t="s">
+      <c r="K72" t="s">
         <v>20</v>
       </c>
-      <c r="L70">
+      <c r="L72">
         <v>2000</v>
       </c>
-      <c r="M70" t="s">
+      <c r="M72" t="s">
         <v>295</v>
       </c>
-      <c r="N70" s="1" t="s">
+      <c r="N72" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="O70" s="6" t="s">
+      <c r="O72" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
-      <c r="A71" s="7"/>
-      <c r="B71" s="9" t="s">
+    <row r="73" spans="1:16">
+      <c r="A73" s="7"/>
+      <c r="B73" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C71" s="9" t="s">
+      <c r="C73" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D71" s="9" t="s">
+      <c r="D73" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E73" t="s">
         <v>201</v>
       </c>
-      <c r="O71" s="6" t="s">
+      <c r="O73" s="6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="O72" s="6" t="s">
+    <row r="74" spans="1:16">
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="O74" s="6" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="O73" s="6"/>
-    </row>
-    <row r="74" spans="1:16">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:16">
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="O75" s="6"/>
+    </row>
+    <row r="76" spans="1:16">
+      <c r="A76" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B76" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="C76" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="D74" s="8" t="s">
+      <c r="D76" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E76" t="s">
         <v>282</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="F76" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G76" t="s">
         <v>11</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H76" t="s">
         <v>76</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I76" t="s">
         <v>9</v>
       </c>
-      <c r="J74" t="s">
+      <c r="J76" t="s">
         <v>67</v>
       </c>
-      <c r="K74" t="s">
+      <c r="K76" t="s">
         <v>20</v>
       </c>
-      <c r="L74">
+      <c r="L76">
         <v>2013</v>
       </c>
-      <c r="M74" t="s">
+      <c r="M76" t="s">
         <v>295</v>
       </c>
-      <c r="N74" s="1" t="s">
+      <c r="N76" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O74" s="6" t="s">
+      <c r="O76" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="P74" s="3" t="s">
+      <c r="P76" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
-      <c r="A75" s="7"/>
-      <c r="B75" s="9" t="s">
+    <row r="77" spans="1:16">
+      <c r="A77" s="7"/>
+      <c r="B77" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C75" s="9" t="s">
+      <c r="C77" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D75" s="9" t="s">
+      <c r="D77" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E75" s="8" t="s">
+      <c r="E77" s="8" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="76" spans="1:16" s="2" customFormat="1">
-      <c r="A76" s="2" t="s">
+    <row r="78" spans="1:16" s="2" customFormat="1">
+      <c r="A78" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="E78" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="F78" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="G78" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H76" s="2" t="s">
+      <c r="H78" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I76" s="2" t="s">
+      <c r="I78" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J76" s="2" t="s">
+      <c r="J78" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K76" s="2" t="s">
+      <c r="K78" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L76" s="2" t="s">
+      <c r="L78" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N76" s="2" t="s">
+      <c r="N78" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O76" s="2" t="s">
+      <c r="O78" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="P76" s="2" t="s">
+      <c r="P78" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
-      <c r="A77" s="1" t="s">
+    <row r="79" spans="1:16">
+      <c r="A79" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="B79" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="C79" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="D77" s="8" t="s">
+      <c r="D79" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E79" t="s">
         <v>248</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="F79" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G77" t="s">
+      <c r="G79" t="s">
         <v>21</v>
       </c>
-      <c r="H77" t="s">
+      <c r="H79" t="s">
         <v>25</v>
       </c>
-      <c r="I77" t="s">
+      <c r="I79" t="s">
         <v>9</v>
       </c>
-      <c r="J77" t="s">
+      <c r="J79" t="s">
         <v>19</v>
       </c>
-      <c r="K77" t="s">
+      <c r="K79" t="s">
         <v>20</v>
       </c>
-      <c r="L77" t="s">
+      <c r="L79" t="s">
         <v>28</v>
       </c>
-      <c r="M77" t="s">
+      <c r="M79" t="s">
         <v>295</v>
       </c>
-      <c r="N77" s="1" t="s">
+      <c r="N79" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O77" s="6" t="s">
+      <c r="O79" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
-      <c r="A78" s="7"/>
-      <c r="B78" s="9" t="s">
+    <row r="80" spans="1:16">
+      <c r="A80" s="7"/>
+      <c r="B80" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C78" s="9" t="s">
+      <c r="C80" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="D80" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E78" s="9" t="s">
+      <c r="E80" s="9" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="79" spans="1:16" s="2" customFormat="1">
-      <c r="A79" s="2" t="s">
+    <row r="81" spans="1:16" s="2" customFormat="1">
+      <c r="A81" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C81" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E81" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F81" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="G81" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H79" s="2" t="s">
+      <c r="H81" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I79" s="2" t="s">
+      <c r="I81" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J79" s="2" t="s">
+      <c r="J81" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K79" s="2" t="s">
+      <c r="K81" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L79" s="2" t="s">
+      <c r="L81" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N79" s="2" t="s">
+      <c r="N81" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O79" s="2" t="s">
+      <c r="O81" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="P79" s="2" t="s">
+      <c r="P81" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
-      <c r="A80" s="1" t="s">
+    <row r="82" spans="1:16">
+      <c r="A82" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B82" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="C80" s="8" t="s">
+      <c r="C82" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="D82" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="E80" s="8" t="s">
+      <c r="E82" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="F80" s="1" t="s">
+      <c r="F82" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G82" t="s">
         <v>21</v>
       </c>
-      <c r="H80" t="s">
+      <c r="H82" t="s">
         <v>25</v>
       </c>
-      <c r="I80" t="s">
+      <c r="I82" t="s">
         <v>9</v>
       </c>
-      <c r="J80" t="s">
+      <c r="J82" t="s">
         <v>72</v>
       </c>
-      <c r="K80" t="s">
+      <c r="K82" t="s">
         <v>27</v>
       </c>
-      <c r="L80" t="s">
+      <c r="L82" t="s">
         <v>28</v>
       </c>
-      <c r="M80" t="s">
+      <c r="M82" t="s">
         <v>295</v>
       </c>
-      <c r="N80" s="1" t="s">
+      <c r="N82" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O80" s="6" t="s">
+      <c r="O82" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
-      <c r="A81" s="7"/>
-      <c r="B81" s="9" t="s">
+    <row r="83" spans="1:16">
+      <c r="A83" s="7"/>
+      <c r="B83" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C81" s="9" t="s">
+      <c r="C83" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="D81" s="9" t="s">
+      <c r="D83" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="E81" s="9" t="s">
+      <c r="E83" s="9" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="83" spans="1:14">
-      <c r="A83" t="s">
+    <row r="85" spans="1:16">
+      <c r="A85" t="s">
         <v>284</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F85" t="s">
         <v>285</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G85" t="s">
         <v>11</v>
       </c>
-      <c r="H83" t="s">
+      <c r="H85" t="s">
         <v>75</v>
       </c>
-      <c r="J83" t="s">
+      <c r="J85" t="s">
         <v>286</v>
       </c>
-      <c r="K83" t="s">
+      <c r="K85" t="s">
         <v>20</v>
       </c>
-      <c r="L83">
+      <c r="L85">
         <v>2000</v>
       </c>
-      <c r="M83" t="s">
+      <c r="M85" t="s">
         <v>295</v>
       </c>
-      <c r="N83" t="s">
+      <c r="N85" t="s">
         <v>287</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1"/>
-    <hyperlink ref="O74" r:id="rId2"/>
-    <hyperlink ref="O65" r:id="rId3"/>
-    <hyperlink ref="O48" r:id="rId4"/>
-    <hyperlink ref="O70" r:id="rId5"/>
-    <hyperlink ref="O32" r:id="rId6"/>
-    <hyperlink ref="O35" r:id="rId7"/>
-    <hyperlink ref="O13" r:id="rId8"/>
-    <hyperlink ref="O16" r:id="rId9"/>
-    <hyperlink ref="O17" r:id="rId10"/>
-    <hyperlink ref="O36" r:id="rId11"/>
-    <hyperlink ref="O66" r:id="rId12"/>
-    <hyperlink ref="O71" r:id="rId13"/>
-    <hyperlink ref="O67" r:id="rId14"/>
-    <hyperlink ref="O72" r:id="rId15"/>
-    <hyperlink ref="O5" r:id="rId16"/>
-    <hyperlink ref="O8" r:id="rId17"/>
-    <hyperlink ref="O10" r:id="rId18"/>
-    <hyperlink ref="O19" r:id="rId19"/>
-    <hyperlink ref="O38" r:id="rId20"/>
-    <hyperlink ref="O42" r:id="rId21"/>
-    <hyperlink ref="O45" r:id="rId22"/>
-    <hyperlink ref="O51" r:id="rId23"/>
-    <hyperlink ref="O54" r:id="rId24"/>
-    <hyperlink ref="O77" r:id="rId25"/>
-    <hyperlink ref="O80" r:id="rId26"/>
-    <hyperlink ref="O39" r:id="rId27"/>
-    <hyperlink ref="O40" r:id="rId28"/>
-    <hyperlink ref="O6" r:id="rId29"/>
-    <hyperlink ref="O24" r:id="rId30"/>
-    <hyperlink ref="O29" r:id="rId31"/>
-    <hyperlink ref="O57" r:id="rId32"/>
-    <hyperlink ref="O62" r:id="rId33"/>
-    <hyperlink ref="O25" r:id="rId34"/>
-    <hyperlink ref="O58" r:id="rId35"/>
-    <hyperlink ref="O26" r:id="rId36"/>
-    <hyperlink ref="O59" r:id="rId37"/>
-    <hyperlink ref="O27" r:id="rId38"/>
-    <hyperlink ref="O60" r:id="rId39"/>
+    <hyperlink ref="O76" r:id="rId2"/>
+    <hyperlink ref="O67" r:id="rId3"/>
+    <hyperlink ref="O50" r:id="rId4"/>
+    <hyperlink ref="O72" r:id="rId5"/>
+    <hyperlink ref="O34" r:id="rId6"/>
+    <hyperlink ref="O37" r:id="rId7"/>
+    <hyperlink ref="O15" r:id="rId8"/>
+    <hyperlink ref="O18" r:id="rId9"/>
+    <hyperlink ref="O19" r:id="rId10"/>
+    <hyperlink ref="O38" r:id="rId11"/>
+    <hyperlink ref="O68" r:id="rId12"/>
+    <hyperlink ref="O73" r:id="rId13"/>
+    <hyperlink ref="O69" r:id="rId14"/>
+    <hyperlink ref="O74" r:id="rId15"/>
+    <hyperlink ref="O7" r:id="rId16"/>
+    <hyperlink ref="O10" r:id="rId17"/>
+    <hyperlink ref="O12" r:id="rId18"/>
+    <hyperlink ref="O21" r:id="rId19"/>
+    <hyperlink ref="O40" r:id="rId20"/>
+    <hyperlink ref="O44" r:id="rId21"/>
+    <hyperlink ref="O47" r:id="rId22"/>
+    <hyperlink ref="O53" r:id="rId23"/>
+    <hyperlink ref="O56" r:id="rId24"/>
+    <hyperlink ref="O79" r:id="rId25"/>
+    <hyperlink ref="O82" r:id="rId26"/>
+    <hyperlink ref="O41" r:id="rId27"/>
+    <hyperlink ref="O42" r:id="rId28"/>
+    <hyperlink ref="O8" r:id="rId29"/>
+    <hyperlink ref="O26" r:id="rId30"/>
+    <hyperlink ref="O31" r:id="rId31"/>
+    <hyperlink ref="O59" r:id="rId32"/>
+    <hyperlink ref="O64" r:id="rId33"/>
+    <hyperlink ref="O27" r:id="rId34"/>
+    <hyperlink ref="O60" r:id="rId35"/>
+    <hyperlink ref="O28" r:id="rId36"/>
+    <hyperlink ref="O61" r:id="rId37"/>
+    <hyperlink ref="O29" r:id="rId38"/>
+    <hyperlink ref="O62" r:id="rId39"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
[dict] changes to comparable texts
</commit_message>
<xml_diff>
--- a/corpus/comparable/metadata.xlsx
+++ b/corpus/comparable/metadata.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25620" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16608" windowHeight="9432" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -1741,25 +1741,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="58.83203125" customWidth="1"/>
-    <col min="3" max="4" width="34.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.796875" customWidth="1"/>
+    <col min="2" max="2" width="58.796875" customWidth="1"/>
+    <col min="3" max="4" width="34.69921875" customWidth="1"/>
     <col min="5" max="5" width="41.5" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.296875" customWidth="1"/>
     <col min="14" max="14" width="63" customWidth="1"/>
-    <col min="15" max="15" width="85.6640625" customWidth="1"/>
+    <col min="15" max="15" width="85.69921875" customWidth="1"/>
     <col min="16" max="16" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1809,7 +1807,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1859,7 +1857,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="9" t="s">
         <v>78</v>
@@ -1874,7 +1872,7 @@
       <c r="O3" s="6"/>
       <c r="P3" s="8"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -1883,7 +1881,7 @@
       <c r="O4" s="6"/>
       <c r="P4" s="8"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>299</v>
       </c>
@@ -1925,14 +1923,14 @@
       <c r="O5" s="6"/>
       <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="O6" s="6"/>
       <c r="P6" s="8"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1982,7 +1980,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -1994,13 +1992,13 @@
       </c>
       <c r="P8" s="8"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="8"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2050,11 +2048,11 @@
         <v>298</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="P11" s="8"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2104,7 +2102,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="9" t="s">
         <v>133</v>
@@ -2119,7 +2117,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="2" customFormat="1">
+    <row r="14" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -2166,7 +2164,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -2213,7 +2211,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="9" t="s">
         <v>102</v>
@@ -2228,12 +2226,12 @@
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -2280,7 +2278,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="9" t="s">
         <v>99</v>
@@ -2298,13 +2296,13 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="O20" s="6"/>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -2351,7 +2349,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="9" t="s">
         <v>130</v>
@@ -2366,10 +2364,10 @@
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -2402,7 +2400,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -2449,7 +2447,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="9" t="s">
         <v>146</v>
@@ -2467,7 +2465,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -2475,7 +2473,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -2483,13 +2481,13 @@
         <v>159</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="O30" s="6"/>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -2539,7 +2537,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="9" t="s">
         <v>143</v>
@@ -2554,7 +2552,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="2" customFormat="1">
+    <row r="33" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>6</v>
       </c>
@@ -2601,7 +2599,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -2651,7 +2649,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35" s="9" t="s">
         <v>93</v>
@@ -2666,12 +2664,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -2721,7 +2719,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="9" t="s">
         <v>96</v>
@@ -2739,13 +2737,13 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="O39" s="6"/>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -2792,7 +2790,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41" s="9" t="s">
         <v>118</v>
@@ -2810,7 +2808,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -2818,12 +2816,12 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -2870,7 +2868,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="7"/>
       <c r="B45" s="9" t="s">
         <v>121</v>
@@ -2885,10 +2883,10 @@
         <v>180</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B46" s="3"/>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -2935,7 +2933,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="7"/>
       <c r="B48" s="9" t="s">
         <v>112</v>
@@ -2950,7 +2948,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="2" customFormat="1">
+    <row r="49" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>6</v>
       </c>
@@ -2997,7 +2995,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -3047,7 +3045,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="7"/>
       <c r="B51" s="9" t="s">
         <v>87</v>
@@ -3062,12 +3060,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -3114,7 +3112,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="7"/>
       <c r="B54" s="9" t="s">
         <v>127</v>
@@ -3129,10 +3127,10 @@
         <v>185</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -3179,7 +3177,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="7"/>
       <c r="B57" s="9" t="s">
         <v>124</v>
@@ -3194,10 +3192,10 @@
         <v>183</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B58" s="3"/>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -3244,7 +3242,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="7"/>
       <c r="B60" s="9" t="s">
         <v>149</v>
@@ -3262,7 +3260,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -3270,7 +3268,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -3278,13 +3276,13 @@
         <v>160</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="O63" s="6"/>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>60</v>
       </c>
@@ -3334,7 +3332,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="7"/>
       <c r="B65" s="9" t="s">
         <v>152</v>
@@ -3349,7 +3347,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="66" spans="1:16" s="2" customFormat="1">
+    <row r="66" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>6</v>
       </c>
@@ -3396,7 +3394,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>62</v>
       </c>
@@ -3444,7 +3442,7 @@
       </c>
       <c r="P67" s="4"/>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="7"/>
       <c r="B68" s="9" t="s">
         <v>84</v>
@@ -3459,7 +3457,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -3467,13 +3465,13 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="O70" s="6"/>
     </row>
-    <row r="71" spans="1:16" s="2" customFormat="1">
+    <row r="71" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>6</v>
       </c>
@@ -3520,7 +3518,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>64</v>
       </c>
@@ -3567,7 +3565,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" s="7"/>
       <c r="B73" s="9" t="s">
         <v>90</v>
@@ -3585,7 +3583,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
@@ -3593,13 +3591,13 @@
         <v>110</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="O75" s="6"/>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>66</v>
       </c>
@@ -3649,7 +3647,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" s="7"/>
       <c r="B77" s="9" t="s">
         <v>81</v>
@@ -3664,7 +3662,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="78" spans="1:16" s="2" customFormat="1">
+    <row r="78" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>6</v>
       </c>
@@ -3711,7 +3709,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>68</v>
       </c>
@@ -3758,7 +3756,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" s="7"/>
       <c r="B80" s="9" t="s">
         <v>115</v>
@@ -3773,7 +3771,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="81" spans="1:16" s="2" customFormat="1">
+    <row r="81" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>6</v>
       </c>
@@ -3820,7 +3818,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>71</v>
       </c>
@@ -3867,7 +3865,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" s="7"/>
       <c r="B83" s="9" t="s">
         <v>136</v>
@@ -3882,7 +3880,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>284</v>
       </c>
@@ -3971,22 +3969,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="75.1640625" customWidth="1"/>
+    <col min="1" max="1" width="75.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>73</v>
       </c>

</xml_diff>